<commit_message>
Bug fix with probabilities
</commit_message>
<xml_diff>
--- a/Data/OurData2.xlsx
+++ b/Data/OurData2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16375D82-10F0-5A45-A682-6414C4EB2B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAD5207-5481-4C42-B21B-0100377D7E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" firstSheet="1" activeTab="2" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
@@ -1537,6 +1537,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1547,15 +1556,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7636,8 +7636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3F5746-A1B1-6F4F-9762-CACD4A91B5F2}">
   <dimension ref="A1:AI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7862,7 +7862,7 @@
         <v>100</v>
       </c>
       <c r="O3" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
@@ -7966,7 +7966,7 @@
         <v>100</v>
       </c>
       <c r="O4" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P4" s="2">
         <v>1</v>
@@ -8072,7 +8072,7 @@
         <v>100</v>
       </c>
       <c r="O5" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P5" s="2">
         <v>1</v>
@@ -8176,7 +8176,7 @@
         <v>100</v>
       </c>
       <c r="O6" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P6" s="2">
         <v>1</v>
@@ -8280,7 +8280,7 @@
         <v>100</v>
       </c>
       <c r="O7" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P7" s="2">
         <v>1</v>
@@ -8386,7 +8386,7 @@
         <v>100</v>
       </c>
       <c r="O8" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P8" s="2">
         <v>1</v>
@@ -8492,7 +8492,7 @@
         <v>100</v>
       </c>
       <c r="O9" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P9" s="2">
         <v>1</v>
@@ -8595,7 +8595,7 @@
         <v>100</v>
       </c>
       <c r="O10" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P10" s="2">
         <v>1</v>
@@ -8699,7 +8699,7 @@
         <v>100</v>
       </c>
       <c r="O11" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P11" s="2">
         <v>1</v>
@@ -8803,7 +8803,7 @@
         <v>100</v>
       </c>
       <c r="O12" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P12" s="2">
         <v>1</v>
@@ -8907,7 +8907,7 @@
         <v>100</v>
       </c>
       <c r="O13" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P13" s="2">
         <v>1</v>
@@ -9011,7 +9011,7 @@
         <v>100</v>
       </c>
       <c r="O14" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P14" s="2">
         <v>1</v>
@@ -9117,7 +9117,7 @@
         <v>100</v>
       </c>
       <c r="O15" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P15" s="2">
         <v>1</v>
@@ -9221,7 +9221,7 @@
         <v>100</v>
       </c>
       <c r="O16" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P16" s="2">
         <v>1</v>
@@ -9325,7 +9325,7 @@
         <v>100</v>
       </c>
       <c r="O17" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P17" s="2">
         <v>1</v>
@@ -9429,7 +9429,7 @@
         <v>100</v>
       </c>
       <c r="O18" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P18" s="2">
         <v>1</v>
@@ -9535,7 +9535,7 @@
         <v>100</v>
       </c>
       <c r="O19" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P19" s="2">
         <v>1</v>
@@ -9641,7 +9641,7 @@
         <v>100</v>
       </c>
       <c r="O20" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P20" s="2">
         <v>1</v>
@@ -9747,7 +9747,7 @@
         <v>100</v>
       </c>
       <c r="O21" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P21" s="2">
         <v>1</v>
@@ -9851,7 +9851,7 @@
         <v>100</v>
       </c>
       <c r="O22" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P22" s="2">
         <v>1</v>
@@ -9957,7 +9957,7 @@
         <v>100</v>
       </c>
       <c r="O23" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P23" s="2">
         <v>1</v>
@@ -10063,7 +10063,7 @@
         <v>100</v>
       </c>
       <c r="O24" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P24" s="2">
         <v>1</v>
@@ -10167,7 +10167,7 @@
         <v>100</v>
       </c>
       <c r="O25" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P25" s="2">
         <v>1</v>
@@ -10271,7 +10271,7 @@
         <v>100</v>
       </c>
       <c r="O26" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P26" s="2">
         <v>1</v>
@@ -10377,7 +10377,7 @@
         <v>100</v>
       </c>
       <c r="O27" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P27" s="2">
         <v>1</v>
@@ -10483,7 +10483,7 @@
         <v>100</v>
       </c>
       <c r="O28" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P28" s="2">
         <v>1</v>
@@ -10589,7 +10589,7 @@
         <v>100</v>
       </c>
       <c r="O29" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P29" s="2">
         <v>1</v>
@@ -10693,7 +10693,7 @@
         <v>100</v>
       </c>
       <c r="O30" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P30" s="2">
         <v>1</v>
@@ -10797,7 +10797,7 @@
         <v>100</v>
       </c>
       <c r="O31" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P31" s="2">
         <v>1</v>
@@ -10901,7 +10901,7 @@
         <v>100</v>
       </c>
       <c r="O32" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P32" s="2">
         <v>1</v>
@@ -11007,7 +11007,7 @@
         <v>100</v>
       </c>
       <c r="O33" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P33" s="2">
         <v>1</v>
@@ -11111,7 +11111,7 @@
         <v>100</v>
       </c>
       <c r="O34" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P34" s="2">
         <v>1</v>
@@ -11215,7 +11215,7 @@
         <v>100</v>
       </c>
       <c r="O35" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P35" s="2">
         <v>1</v>
@@ -11321,7 +11321,7 @@
         <v>100</v>
       </c>
       <c r="O36" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P36" s="2">
         <v>1</v>
@@ -11427,7 +11427,7 @@
         <v>100</v>
       </c>
       <c r="O37" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P37" s="2">
         <v>1</v>
@@ -11531,7 +11531,7 @@
         <v>100</v>
       </c>
       <c r="O38" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P38" s="2">
         <v>1</v>
@@ -11635,7 +11635,7 @@
         <v>100</v>
       </c>
       <c r="O39" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P39" s="2">
         <v>1</v>
@@ -11739,7 +11739,7 @@
         <v>100</v>
       </c>
       <c r="O40" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P40" s="2">
         <v>1</v>
@@ -11845,7 +11845,7 @@
         <v>100</v>
       </c>
       <c r="O41" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P41" s="2">
         <v>1</v>
@@ -11949,7 +11949,7 @@
         <v>100</v>
       </c>
       <c r="O42" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P42" s="2">
         <v>1</v>
@@ -12055,7 +12055,7 @@
         <v>100</v>
       </c>
       <c r="O43" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P43" s="2">
         <v>1</v>
@@ -12161,7 +12161,7 @@
         <v>100</v>
       </c>
       <c r="O44" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P44" s="2">
         <v>1</v>
@@ -12265,7 +12265,7 @@
         <v>100</v>
       </c>
       <c r="O45" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P45" s="2">
         <v>1</v>
@@ -12369,7 +12369,7 @@
         <v>100</v>
       </c>
       <c r="O46" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P46" s="2">
         <v>1</v>
@@ -12473,7 +12473,7 @@
         <v>100</v>
       </c>
       <c r="O47" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P47" s="2">
         <v>1</v>
@@ -12577,7 +12577,7 @@
         <v>100</v>
       </c>
       <c r="O48" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P48" s="2">
         <v>1</v>
@@ -12683,7 +12683,7 @@
         <v>100</v>
       </c>
       <c r="O49" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P49" s="2">
         <v>1</v>
@@ -12789,7 +12789,7 @@
         <v>100</v>
       </c>
       <c r="O50" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P50" s="2">
         <v>1</v>
@@ -12895,7 +12895,7 @@
         <v>100</v>
       </c>
       <c r="O51" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P51" s="2">
         <v>1</v>
@@ -12999,7 +12999,7 @@
         <v>100</v>
       </c>
       <c r="O52" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P52" s="2">
         <v>1</v>
@@ -13103,7 +13103,7 @@
         <v>100</v>
       </c>
       <c r="O53" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P53" s="2">
         <v>1</v>
@@ -13209,7 +13209,7 @@
         <v>100</v>
       </c>
       <c r="O54" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P54" s="2">
         <v>1</v>
@@ -13313,7 +13313,7 @@
         <v>100</v>
       </c>
       <c r="O55" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P55" s="2">
         <v>1</v>
@@ -13417,7 +13417,7 @@
         <v>100</v>
       </c>
       <c r="O56" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P56" s="2">
         <v>1</v>
@@ -13523,7 +13523,7 @@
         <v>100</v>
       </c>
       <c r="O57" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P57" s="2">
         <v>1</v>
@@ -13629,7 +13629,7 @@
         <v>100</v>
       </c>
       <c r="O58" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P58" s="2">
         <v>1</v>
@@ -13733,7 +13733,7 @@
         <v>100</v>
       </c>
       <c r="O59" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P59" s="2">
         <v>1</v>
@@ -13839,7 +13839,7 @@
         <v>100</v>
       </c>
       <c r="O60" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P60" s="2">
         <v>1</v>
@@ -13943,7 +13943,7 @@
         <v>100</v>
       </c>
       <c r="O61" s="2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="P61" s="2">
         <v>1</v>
@@ -14858,7 +14858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19292E87-5CF7-794D-A1AA-7C1926221C7B}">
   <dimension ref="A1:BM54"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -18297,6 +18297,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AG3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AH2:AW2"/>
     <mergeCell ref="AH3:AO3"/>
@@ -18305,14 +18313,6 @@
     <mergeCell ref="AX2:BM2"/>
     <mergeCell ref="AX3:BE3"/>
     <mergeCell ref="BF3:BM3"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18954,294 +18954,294 @@
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="60">
-        <v>5</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="60">
-        <v>5</v>
-      </c>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="61"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="61"/>
-      <c r="AG3" s="62"/>
-      <c r="AH3" s="60">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="61"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="61"/>
-      <c r="AL3" s="61"/>
-      <c r="AM3" s="61"/>
-      <c r="AN3" s="61"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="61"/>
-      <c r="AQ3" s="61"/>
-      <c r="AR3" s="61"/>
-      <c r="AS3" s="61"/>
-      <c r="AT3" s="61"/>
-      <c r="AU3" s="61"/>
-      <c r="AV3" s="61"/>
-      <c r="AW3" s="62"/>
-      <c r="AX3" s="60">
-        <v>5</v>
-      </c>
-      <c r="AY3" s="61"/>
-      <c r="AZ3" s="61"/>
-      <c r="BA3" s="61"/>
-      <c r="BB3" s="61"/>
-      <c r="BC3" s="61"/>
-      <c r="BD3" s="61"/>
-      <c r="BE3" s="61"/>
-      <c r="BF3" s="61"/>
-      <c r="BG3" s="61"/>
-      <c r="BH3" s="61"/>
-      <c r="BI3" s="61"/>
-      <c r="BJ3" s="61"/>
-      <c r="BK3" s="61"/>
-      <c r="BL3" s="61"/>
-      <c r="BM3" s="62"/>
-      <c r="BN3" s="60">
+      <c r="B3" s="63">
+        <v>5</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="63">
+        <v>5</v>
+      </c>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="63">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+      <c r="AV3" s="64"/>
+      <c r="AW3" s="65"/>
+      <c r="AX3" s="63">
+        <v>5</v>
+      </c>
+      <c r="AY3" s="64"/>
+      <c r="AZ3" s="64"/>
+      <c r="BA3" s="64"/>
+      <c r="BB3" s="64"/>
+      <c r="BC3" s="64"/>
+      <c r="BD3" s="64"/>
+      <c r="BE3" s="64"/>
+      <c r="BF3" s="64"/>
+      <c r="BG3" s="64"/>
+      <c r="BH3" s="64"/>
+      <c r="BI3" s="64"/>
+      <c r="BJ3" s="64"/>
+      <c r="BK3" s="64"/>
+      <c r="BL3" s="64"/>
+      <c r="BM3" s="65"/>
+      <c r="BN3" s="63">
         <v>9</v>
       </c>
-      <c r="BO3" s="61"/>
-      <c r="BP3" s="61"/>
-      <c r="BQ3" s="61"/>
-      <c r="BR3" s="61"/>
-      <c r="BS3" s="61"/>
-      <c r="BT3" s="61"/>
-      <c r="BU3" s="61"/>
-      <c r="BV3" s="61"/>
-      <c r="BW3" s="61"/>
-      <c r="BX3" s="61"/>
-      <c r="BY3" s="61"/>
-      <c r="BZ3" s="61"/>
-      <c r="CA3" s="61"/>
-      <c r="CB3" s="61"/>
-      <c r="CC3" s="62"/>
-      <c r="CD3" s="60">
+      <c r="BO3" s="64"/>
+      <c r="BP3" s="64"/>
+      <c r="BQ3" s="64"/>
+      <c r="BR3" s="64"/>
+      <c r="BS3" s="64"/>
+      <c r="BT3" s="64"/>
+      <c r="BU3" s="64"/>
+      <c r="BV3" s="64"/>
+      <c r="BW3" s="64"/>
+      <c r="BX3" s="64"/>
+      <c r="BY3" s="64"/>
+      <c r="BZ3" s="64"/>
+      <c r="CA3" s="64"/>
+      <c r="CB3" s="64"/>
+      <c r="CC3" s="65"/>
+      <c r="CD3" s="63">
         <v>9</v>
       </c>
-      <c r="CE3" s="61"/>
-      <c r="CF3" s="61"/>
-      <c r="CG3" s="61"/>
-      <c r="CH3" s="61"/>
-      <c r="CI3" s="61"/>
-      <c r="CJ3" s="61"/>
-      <c r="CK3" s="61"/>
-      <c r="CL3" s="61"/>
-      <c r="CM3" s="61"/>
-      <c r="CN3" s="61"/>
-      <c r="CO3" s="61"/>
-      <c r="CP3" s="61"/>
-      <c r="CQ3" s="61"/>
-      <c r="CR3" s="61"/>
-      <c r="CS3" s="62"/>
-      <c r="CT3" s="60">
+      <c r="CE3" s="64"/>
+      <c r="CF3" s="64"/>
+      <c r="CG3" s="64"/>
+      <c r="CH3" s="64"/>
+      <c r="CI3" s="64"/>
+      <c r="CJ3" s="64"/>
+      <c r="CK3" s="64"/>
+      <c r="CL3" s="64"/>
+      <c r="CM3" s="64"/>
+      <c r="CN3" s="64"/>
+      <c r="CO3" s="64"/>
+      <c r="CP3" s="64"/>
+      <c r="CQ3" s="64"/>
+      <c r="CR3" s="64"/>
+      <c r="CS3" s="65"/>
+      <c r="CT3" s="63">
         <v>9</v>
       </c>
-      <c r="CU3" s="61"/>
-      <c r="CV3" s="61"/>
-      <c r="CW3" s="61"/>
-      <c r="CX3" s="61"/>
-      <c r="CY3" s="61"/>
-      <c r="CZ3" s="61"/>
-      <c r="DA3" s="61"/>
-      <c r="DB3" s="61"/>
-      <c r="DC3" s="61"/>
-      <c r="DD3" s="61"/>
-      <c r="DE3" s="61"/>
-      <c r="DF3" s="61"/>
-      <c r="DG3" s="61"/>
-      <c r="DH3" s="61"/>
-      <c r="DI3" s="62"/>
-      <c r="DJ3" s="60">
+      <c r="CU3" s="64"/>
+      <c r="CV3" s="64"/>
+      <c r="CW3" s="64"/>
+      <c r="CX3" s="64"/>
+      <c r="CY3" s="64"/>
+      <c r="CZ3" s="64"/>
+      <c r="DA3" s="64"/>
+      <c r="DB3" s="64"/>
+      <c r="DC3" s="64"/>
+      <c r="DD3" s="64"/>
+      <c r="DE3" s="64"/>
+      <c r="DF3" s="64"/>
+      <c r="DG3" s="64"/>
+      <c r="DH3" s="64"/>
+      <c r="DI3" s="65"/>
+      <c r="DJ3" s="63">
         <v>9</v>
       </c>
-      <c r="DK3" s="61"/>
-      <c r="DL3" s="61"/>
-      <c r="DM3" s="61"/>
-      <c r="DN3" s="61"/>
-      <c r="DO3" s="61"/>
-      <c r="DP3" s="61"/>
-      <c r="DQ3" s="61"/>
-      <c r="DR3" s="61"/>
-      <c r="DS3" s="61"/>
-      <c r="DT3" s="61"/>
-      <c r="DU3" s="61"/>
-      <c r="DV3" s="61"/>
-      <c r="DW3" s="61"/>
-      <c r="DX3" s="61"/>
-      <c r="DY3" s="62"/>
-      <c r="DZ3" s="63">
+      <c r="DK3" s="64"/>
+      <c r="DL3" s="64"/>
+      <c r="DM3" s="64"/>
+      <c r="DN3" s="64"/>
+      <c r="DO3" s="64"/>
+      <c r="DP3" s="64"/>
+      <c r="DQ3" s="64"/>
+      <c r="DR3" s="64"/>
+      <c r="DS3" s="64"/>
+      <c r="DT3" s="64"/>
+      <c r="DU3" s="64"/>
+      <c r="DV3" s="64"/>
+      <c r="DW3" s="64"/>
+      <c r="DX3" s="64"/>
+      <c r="DY3" s="65"/>
+      <c r="DZ3" s="66">
         <v>13</v>
       </c>
-      <c r="EA3" s="64"/>
-      <c r="EB3" s="64"/>
-      <c r="EC3" s="64"/>
-      <c r="ED3" s="64"/>
-      <c r="EE3" s="64"/>
-      <c r="EF3" s="64"/>
-      <c r="EG3" s="64"/>
-      <c r="EH3" s="64"/>
-      <c r="EI3" s="64"/>
-      <c r="EJ3" s="64"/>
-      <c r="EK3" s="64"/>
-      <c r="EL3" s="64"/>
-      <c r="EM3" s="64"/>
-      <c r="EN3" s="64"/>
-      <c r="EO3" s="65"/>
-      <c r="EP3" s="66">
+      <c r="EA3" s="61"/>
+      <c r="EB3" s="61"/>
+      <c r="EC3" s="61"/>
+      <c r="ED3" s="61"/>
+      <c r="EE3" s="61"/>
+      <c r="EF3" s="61"/>
+      <c r="EG3" s="61"/>
+      <c r="EH3" s="61"/>
+      <c r="EI3" s="61"/>
+      <c r="EJ3" s="61"/>
+      <c r="EK3" s="61"/>
+      <c r="EL3" s="61"/>
+      <c r="EM3" s="61"/>
+      <c r="EN3" s="61"/>
+      <c r="EO3" s="62"/>
+      <c r="EP3" s="60">
         <v>13</v>
       </c>
-      <c r="EQ3" s="64"/>
-      <c r="ER3" s="64"/>
-      <c r="ES3" s="64"/>
-      <c r="ET3" s="64"/>
-      <c r="EU3" s="64"/>
-      <c r="EV3" s="64"/>
-      <c r="EW3" s="64"/>
-      <c r="EX3" s="64"/>
-      <c r="EY3" s="64"/>
-      <c r="EZ3" s="64"/>
-      <c r="FA3" s="64"/>
-      <c r="FB3" s="64"/>
-      <c r="FC3" s="64"/>
-      <c r="FD3" s="64"/>
-      <c r="FE3" s="65"/>
-      <c r="FF3" s="66">
+      <c r="EQ3" s="61"/>
+      <c r="ER3" s="61"/>
+      <c r="ES3" s="61"/>
+      <c r="ET3" s="61"/>
+      <c r="EU3" s="61"/>
+      <c r="EV3" s="61"/>
+      <c r="EW3" s="61"/>
+      <c r="EX3" s="61"/>
+      <c r="EY3" s="61"/>
+      <c r="EZ3" s="61"/>
+      <c r="FA3" s="61"/>
+      <c r="FB3" s="61"/>
+      <c r="FC3" s="61"/>
+      <c r="FD3" s="61"/>
+      <c r="FE3" s="62"/>
+      <c r="FF3" s="60">
         <v>13</v>
       </c>
-      <c r="FG3" s="64"/>
-      <c r="FH3" s="64"/>
-      <c r="FI3" s="64"/>
-      <c r="FJ3" s="64"/>
-      <c r="FK3" s="64"/>
-      <c r="FL3" s="64"/>
-      <c r="FM3" s="64"/>
-      <c r="FN3" s="64"/>
-      <c r="FO3" s="64"/>
-      <c r="FP3" s="64"/>
-      <c r="FQ3" s="64"/>
-      <c r="FR3" s="64"/>
-      <c r="FS3" s="64"/>
-      <c r="FT3" s="64"/>
-      <c r="FU3" s="65"/>
-      <c r="FV3" s="66">
+      <c r="FG3" s="61"/>
+      <c r="FH3" s="61"/>
+      <c r="FI3" s="61"/>
+      <c r="FJ3" s="61"/>
+      <c r="FK3" s="61"/>
+      <c r="FL3" s="61"/>
+      <c r="FM3" s="61"/>
+      <c r="FN3" s="61"/>
+      <c r="FO3" s="61"/>
+      <c r="FP3" s="61"/>
+      <c r="FQ3" s="61"/>
+      <c r="FR3" s="61"/>
+      <c r="FS3" s="61"/>
+      <c r="FT3" s="61"/>
+      <c r="FU3" s="62"/>
+      <c r="FV3" s="60">
         <v>13</v>
       </c>
-      <c r="FW3" s="64"/>
-      <c r="FX3" s="64"/>
-      <c r="FY3" s="64"/>
-      <c r="FZ3" s="64"/>
-      <c r="GA3" s="64"/>
-      <c r="GB3" s="64"/>
-      <c r="GC3" s="64"/>
-      <c r="GD3" s="64"/>
-      <c r="GE3" s="64"/>
-      <c r="GF3" s="64"/>
-      <c r="GG3" s="64"/>
-      <c r="GH3" s="64"/>
-      <c r="GI3" s="64"/>
-      <c r="GJ3" s="64"/>
-      <c r="GK3" s="65"/>
-      <c r="GL3" s="66">
+      <c r="FW3" s="61"/>
+      <c r="FX3" s="61"/>
+      <c r="FY3" s="61"/>
+      <c r="FZ3" s="61"/>
+      <c r="GA3" s="61"/>
+      <c r="GB3" s="61"/>
+      <c r="GC3" s="61"/>
+      <c r="GD3" s="61"/>
+      <c r="GE3" s="61"/>
+      <c r="GF3" s="61"/>
+      <c r="GG3" s="61"/>
+      <c r="GH3" s="61"/>
+      <c r="GI3" s="61"/>
+      <c r="GJ3" s="61"/>
+      <c r="GK3" s="62"/>
+      <c r="GL3" s="60">
         <v>17</v>
       </c>
-      <c r="GM3" s="64"/>
-      <c r="GN3" s="64"/>
-      <c r="GO3" s="64"/>
-      <c r="GP3" s="64"/>
-      <c r="GQ3" s="64"/>
-      <c r="GR3" s="64"/>
-      <c r="GS3" s="64"/>
-      <c r="GT3" s="64"/>
-      <c r="GU3" s="64"/>
-      <c r="GV3" s="64"/>
-      <c r="GW3" s="64"/>
-      <c r="GX3" s="64"/>
-      <c r="GY3" s="64"/>
-      <c r="GZ3" s="64"/>
-      <c r="HA3" s="65"/>
-      <c r="HB3" s="66">
+      <c r="GM3" s="61"/>
+      <c r="GN3" s="61"/>
+      <c r="GO3" s="61"/>
+      <c r="GP3" s="61"/>
+      <c r="GQ3" s="61"/>
+      <c r="GR3" s="61"/>
+      <c r="GS3" s="61"/>
+      <c r="GT3" s="61"/>
+      <c r="GU3" s="61"/>
+      <c r="GV3" s="61"/>
+      <c r="GW3" s="61"/>
+      <c r="GX3" s="61"/>
+      <c r="GY3" s="61"/>
+      <c r="GZ3" s="61"/>
+      <c r="HA3" s="62"/>
+      <c r="HB3" s="60">
         <v>17</v>
       </c>
-      <c r="HC3" s="64"/>
-      <c r="HD3" s="64"/>
-      <c r="HE3" s="64"/>
-      <c r="HF3" s="64"/>
-      <c r="HG3" s="64"/>
-      <c r="HH3" s="64"/>
-      <c r="HI3" s="64"/>
-      <c r="HJ3" s="64"/>
-      <c r="HK3" s="64"/>
-      <c r="HL3" s="64"/>
-      <c r="HM3" s="64"/>
-      <c r="HN3" s="64"/>
-      <c r="HO3" s="64"/>
-      <c r="HP3" s="64"/>
-      <c r="HQ3" s="65"/>
-      <c r="HR3" s="66">
+      <c r="HC3" s="61"/>
+      <c r="HD3" s="61"/>
+      <c r="HE3" s="61"/>
+      <c r="HF3" s="61"/>
+      <c r="HG3" s="61"/>
+      <c r="HH3" s="61"/>
+      <c r="HI3" s="61"/>
+      <c r="HJ3" s="61"/>
+      <c r="HK3" s="61"/>
+      <c r="HL3" s="61"/>
+      <c r="HM3" s="61"/>
+      <c r="HN3" s="61"/>
+      <c r="HO3" s="61"/>
+      <c r="HP3" s="61"/>
+      <c r="HQ3" s="62"/>
+      <c r="HR3" s="60">
         <v>17</v>
       </c>
-      <c r="HS3" s="64"/>
-      <c r="HT3" s="64"/>
-      <c r="HU3" s="64"/>
-      <c r="HV3" s="64"/>
-      <c r="HW3" s="64"/>
-      <c r="HX3" s="64"/>
-      <c r="HY3" s="64"/>
-      <c r="HZ3" s="64"/>
-      <c r="IA3" s="64"/>
-      <c r="IB3" s="64"/>
-      <c r="IC3" s="64"/>
-      <c r="ID3" s="64"/>
-      <c r="IE3" s="64"/>
-      <c r="IF3" s="64"/>
-      <c r="IG3" s="65"/>
-      <c r="IH3" s="66">
+      <c r="HS3" s="61"/>
+      <c r="HT3" s="61"/>
+      <c r="HU3" s="61"/>
+      <c r="HV3" s="61"/>
+      <c r="HW3" s="61"/>
+      <c r="HX3" s="61"/>
+      <c r="HY3" s="61"/>
+      <c r="HZ3" s="61"/>
+      <c r="IA3" s="61"/>
+      <c r="IB3" s="61"/>
+      <c r="IC3" s="61"/>
+      <c r="ID3" s="61"/>
+      <c r="IE3" s="61"/>
+      <c r="IF3" s="61"/>
+      <c r="IG3" s="62"/>
+      <c r="IH3" s="60">
         <v>17</v>
       </c>
-      <c r="II3" s="64"/>
-      <c r="IJ3" s="64"/>
-      <c r="IK3" s="64"/>
-      <c r="IL3" s="64"/>
-      <c r="IM3" s="64"/>
-      <c r="IN3" s="64"/>
-      <c r="IO3" s="64"/>
-      <c r="IP3" s="64"/>
-      <c r="IQ3" s="64"/>
-      <c r="IR3" s="64"/>
-      <c r="IS3" s="64"/>
-      <c r="IT3" s="64"/>
-      <c r="IU3" s="64"/>
-      <c r="IV3" s="64"/>
-      <c r="IW3" s="65"/>
+      <c r="II3" s="61"/>
+      <c r="IJ3" s="61"/>
+      <c r="IK3" s="61"/>
+      <c r="IL3" s="61"/>
+      <c r="IM3" s="61"/>
+      <c r="IN3" s="61"/>
+      <c r="IO3" s="61"/>
+      <c r="IP3" s="61"/>
+      <c r="IQ3" s="61"/>
+      <c r="IR3" s="61"/>
+      <c r="IS3" s="61"/>
+      <c r="IT3" s="61"/>
+      <c r="IU3" s="61"/>
+      <c r="IV3" s="61"/>
+      <c r="IW3" s="62"/>
     </row>
     <row r="4" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -29942,19 +29942,57 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="HB2:HQ2"/>
-    <mergeCell ref="HR2:IG2"/>
-    <mergeCell ref="IH2:IW2"/>
-    <mergeCell ref="DZ2:EO2"/>
-    <mergeCell ref="EP2:FE2"/>
-    <mergeCell ref="FF2:FU2"/>
-    <mergeCell ref="FV2:GK2"/>
-    <mergeCell ref="GL2:HA2"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="BN2:CC2"/>
-    <mergeCell ref="CD2:CS2"/>
-    <mergeCell ref="CT2:DI2"/>
-    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AH4:AO4"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="BN4:BU4"/>
+    <mergeCell ref="BV4:CC4"/>
+    <mergeCell ref="CD4:CK4"/>
+    <mergeCell ref="CL4:CS4"/>
+    <mergeCell ref="CT4:DA4"/>
+    <mergeCell ref="DB4:DI4"/>
+    <mergeCell ref="DJ4:DQ4"/>
+    <mergeCell ref="DR4:DY4"/>
+    <mergeCell ref="DZ4:EG4"/>
+    <mergeCell ref="EH4:EO4"/>
+    <mergeCell ref="EP4:EW4"/>
+    <mergeCell ref="EX4:FE4"/>
+    <mergeCell ref="FF4:FM4"/>
+    <mergeCell ref="FN4:FU4"/>
+    <mergeCell ref="FV4:GC4"/>
+    <mergeCell ref="GD4:GK4"/>
+    <mergeCell ref="GL4:GS4"/>
+    <mergeCell ref="GT4:HA4"/>
+    <mergeCell ref="HB4:HI4"/>
+    <mergeCell ref="HJ4:HQ4"/>
+    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="HZ4:IG4"/>
+    <mergeCell ref="IH4:IO4"/>
+    <mergeCell ref="IP4:IW4"/>
+    <mergeCell ref="AH3:AW3"/>
+    <mergeCell ref="AX3:BM3"/>
+    <mergeCell ref="BN3:CC3"/>
+    <mergeCell ref="CD3:CS3"/>
+    <mergeCell ref="CT3:DI3"/>
+    <mergeCell ref="DJ3:DY3"/>
+    <mergeCell ref="DZ3:EO3"/>
+    <mergeCell ref="EP3:FE3"/>
+    <mergeCell ref="FF3:FU3"/>
+    <mergeCell ref="FV3:GK3"/>
+    <mergeCell ref="GL3:HA3"/>
+    <mergeCell ref="HB3:HQ3"/>
+    <mergeCell ref="HR3:IG3"/>
     <mergeCell ref="IH3:IW3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AX1:BM1"/>
@@ -29971,57 +30009,19 @@
     <mergeCell ref="HR1:IG1"/>
     <mergeCell ref="IH1:IW1"/>
     <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="HZ4:IG4"/>
-    <mergeCell ref="IH4:IO4"/>
-    <mergeCell ref="IP4:IW4"/>
-    <mergeCell ref="AH3:AW3"/>
-    <mergeCell ref="AX3:BM3"/>
-    <mergeCell ref="BN3:CC3"/>
-    <mergeCell ref="CD3:CS3"/>
-    <mergeCell ref="CT3:DI3"/>
-    <mergeCell ref="DJ3:DY3"/>
-    <mergeCell ref="DZ3:EO3"/>
-    <mergeCell ref="EP3:FE3"/>
-    <mergeCell ref="FF3:FU3"/>
-    <mergeCell ref="FV3:GK3"/>
-    <mergeCell ref="GL3:HA3"/>
-    <mergeCell ref="HB3:HQ3"/>
-    <mergeCell ref="HR3:IG3"/>
-    <mergeCell ref="GL4:GS4"/>
-    <mergeCell ref="GT4:HA4"/>
-    <mergeCell ref="HB4:HI4"/>
-    <mergeCell ref="HJ4:HQ4"/>
-    <mergeCell ref="HR4:HY4"/>
-    <mergeCell ref="EX4:FE4"/>
-    <mergeCell ref="FF4:FM4"/>
-    <mergeCell ref="FN4:FU4"/>
-    <mergeCell ref="FV4:GC4"/>
-    <mergeCell ref="GD4:GK4"/>
-    <mergeCell ref="DJ4:DQ4"/>
-    <mergeCell ref="DR4:DY4"/>
-    <mergeCell ref="DZ4:EG4"/>
-    <mergeCell ref="EH4:EO4"/>
-    <mergeCell ref="EP4:EW4"/>
-    <mergeCell ref="BV4:CC4"/>
-    <mergeCell ref="CD4:CK4"/>
-    <mergeCell ref="CL4:CS4"/>
-    <mergeCell ref="CT4:DA4"/>
-    <mergeCell ref="DB4:DI4"/>
-    <mergeCell ref="AH4:AO4"/>
-    <mergeCell ref="AP4:AW4"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="BF4:BM4"/>
-    <mergeCell ref="BN4:BU4"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="BN2:CC2"/>
+    <mergeCell ref="CD2:CS2"/>
+    <mergeCell ref="CT2:DI2"/>
+    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="HB2:HQ2"/>
+    <mergeCell ref="HR2:IG2"/>
+    <mergeCell ref="IH2:IW2"/>
+    <mergeCell ref="DZ2:EO2"/>
+    <mergeCell ref="EP2:FE2"/>
+    <mergeCell ref="FF2:FU2"/>
+    <mergeCell ref="FV2:GK2"/>
+    <mergeCell ref="GL2:HA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Eerste versie manuscript af
</commit_message>
<xml_diff>
--- a/Data/OurData2.xlsx
+++ b/Data/OurData2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902E0F22-6231-D544-BB08-4E3DD6D6694D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CD28D3-87F6-F74D-AA19-039383E25C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" firstSheet="1" activeTab="2" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
+    <workbookView xWindow="1300" yWindow="500" windowWidth="28800" windowHeight="16060" firstSheet="1" activeTab="11" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualisation" sheetId="7" r:id="rId1"/>
@@ -34,6 +34,41 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Arcs!$A$1:$N$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Nodes!$A$2:$AI$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">ProductionCapacities!$A$1:$H$51</definedName>
+    <definedName name="solver_adj" localSheetId="11" hidden="1">TraderPercentages!$B$2:$I$9</definedName>
+    <definedName name="solver_cvg" localSheetId="11" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="11" hidden="1">TraderPercentages!$D$2:$D$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="11" hidden="1">TraderPercentages!$D$6:$D$9</definedName>
+    <definedName name="solver_lhs3" localSheetId="11" hidden="1">TraderPercentages!$L$2:$L$9</definedName>
+    <definedName name="solver_lin" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="11" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="11" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="11" hidden="1">3</definedName>
+    <definedName name="solver_opt" localSheetId="11" hidden="1">TraderPercentages!$L$10</definedName>
+    <definedName name="solver_pre" localSheetId="11" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="11" hidden="1">TraderPercentages!$K$2:$K$9</definedName>
+    <definedName name="solver_rlx" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="11" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="11" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="11" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1552,6 +1587,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1562,15 +1606,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1957,7 +1992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902688A-D2A3-854F-B341-C0BEC53AF991}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -5709,8 +5744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7B38E3-302C-2E43-9786-274195CEF373}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5724,8 +5759,8 @@
     <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -5768,25 +5803,25 @@
         <v>172</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -5797,7 +5832,7 @@
       </c>
       <c r="L2" cm="1">
         <f t="array" ref="L2">SUM(B2:I2*MAX('Demand Stage 1'!$B$5:$I$8))</f>
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -5879,28 +5914,28 @@
         <v>163</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f>HLOOKUP(A5,Traders!$A$1:$H$15,15,)</f>
@@ -5908,7 +5943,7 @@
       </c>
       <c r="L5" cm="1">
         <f t="array" ref="L5">SUM(B5:I5*MAX('Demand Stage 1'!$B$5:$I$8))</f>
-        <v>0</v>
+        <v>292.5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -6026,28 +6061,28 @@
       <c r="A9" s="40" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="40">
-        <v>0</v>
-      </c>
-      <c r="C9" s="40">
-        <v>0</v>
-      </c>
-      <c r="D9" s="40">
-        <v>0</v>
-      </c>
-      <c r="E9" s="40">
-        <v>0</v>
-      </c>
-      <c r="F9" s="40">
-        <v>0</v>
-      </c>
-      <c r="G9" s="40">
-        <v>0</v>
-      </c>
-      <c r="H9" s="40">
-        <v>0</v>
-      </c>
-      <c r="I9" s="40">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>0</v>
       </c>
       <c r="J9" s="40"/>
@@ -6066,39 +6101,39 @@
       </c>
       <c r="B10">
         <f>SUM(B2:B9)</f>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:I10" si="0">SUM(C2:C9)</f>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(E2:E9)</f>
+        <v>0.95</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(F2:F9)</f>
+        <v>0.95</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="H10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" cm="1">
         <f t="array" ref="L10">SUM(B10:I10*MAX('Demand Stage 1'!$B$5:$I$8))</f>
-        <v>0</v>
+        <v>346.5</v>
       </c>
     </row>
   </sheetData>
@@ -7671,7 +7706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3F5746-A1B1-6F4F-9762-CACD4A91B5F2}">
   <dimension ref="A1:AI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
@@ -18332,6 +18367,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AG3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AH2:AW2"/>
     <mergeCell ref="AH3:AO3"/>
@@ -18340,14 +18383,6 @@
     <mergeCell ref="AX2:BM2"/>
     <mergeCell ref="AX3:BE3"/>
     <mergeCell ref="BF3:BM3"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18989,294 +19024,294 @@
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="60">
-        <v>5</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="60">
-        <v>5</v>
-      </c>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="61"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="61"/>
-      <c r="AG3" s="62"/>
-      <c r="AH3" s="60">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="61"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="61"/>
-      <c r="AL3" s="61"/>
-      <c r="AM3" s="61"/>
-      <c r="AN3" s="61"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="61"/>
-      <c r="AQ3" s="61"/>
-      <c r="AR3" s="61"/>
-      <c r="AS3" s="61"/>
-      <c r="AT3" s="61"/>
-      <c r="AU3" s="61"/>
-      <c r="AV3" s="61"/>
-      <c r="AW3" s="62"/>
-      <c r="AX3" s="60">
-        <v>5</v>
-      </c>
-      <c r="AY3" s="61"/>
-      <c r="AZ3" s="61"/>
-      <c r="BA3" s="61"/>
-      <c r="BB3" s="61"/>
-      <c r="BC3" s="61"/>
-      <c r="BD3" s="61"/>
-      <c r="BE3" s="61"/>
-      <c r="BF3" s="61"/>
-      <c r="BG3" s="61"/>
-      <c r="BH3" s="61"/>
-      <c r="BI3" s="61"/>
-      <c r="BJ3" s="61"/>
-      <c r="BK3" s="61"/>
-      <c r="BL3" s="61"/>
-      <c r="BM3" s="62"/>
-      <c r="BN3" s="60">
+      <c r="B3" s="63">
+        <v>5</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="63">
+        <v>5</v>
+      </c>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="63">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+      <c r="AV3" s="64"/>
+      <c r="AW3" s="65"/>
+      <c r="AX3" s="63">
+        <v>5</v>
+      </c>
+      <c r="AY3" s="64"/>
+      <c r="AZ3" s="64"/>
+      <c r="BA3" s="64"/>
+      <c r="BB3" s="64"/>
+      <c r="BC3" s="64"/>
+      <c r="BD3" s="64"/>
+      <c r="BE3" s="64"/>
+      <c r="BF3" s="64"/>
+      <c r="BG3" s="64"/>
+      <c r="BH3" s="64"/>
+      <c r="BI3" s="64"/>
+      <c r="BJ3" s="64"/>
+      <c r="BK3" s="64"/>
+      <c r="BL3" s="64"/>
+      <c r="BM3" s="65"/>
+      <c r="BN3" s="63">
         <v>9</v>
       </c>
-      <c r="BO3" s="61"/>
-      <c r="BP3" s="61"/>
-      <c r="BQ3" s="61"/>
-      <c r="BR3" s="61"/>
-      <c r="BS3" s="61"/>
-      <c r="BT3" s="61"/>
-      <c r="BU3" s="61"/>
-      <c r="BV3" s="61"/>
-      <c r="BW3" s="61"/>
-      <c r="BX3" s="61"/>
-      <c r="BY3" s="61"/>
-      <c r="BZ3" s="61"/>
-      <c r="CA3" s="61"/>
-      <c r="CB3" s="61"/>
-      <c r="CC3" s="62"/>
-      <c r="CD3" s="60">
+      <c r="BO3" s="64"/>
+      <c r="BP3" s="64"/>
+      <c r="BQ3" s="64"/>
+      <c r="BR3" s="64"/>
+      <c r="BS3" s="64"/>
+      <c r="BT3" s="64"/>
+      <c r="BU3" s="64"/>
+      <c r="BV3" s="64"/>
+      <c r="BW3" s="64"/>
+      <c r="BX3" s="64"/>
+      <c r="BY3" s="64"/>
+      <c r="BZ3" s="64"/>
+      <c r="CA3" s="64"/>
+      <c r="CB3" s="64"/>
+      <c r="CC3" s="65"/>
+      <c r="CD3" s="63">
         <v>9</v>
       </c>
-      <c r="CE3" s="61"/>
-      <c r="CF3" s="61"/>
-      <c r="CG3" s="61"/>
-      <c r="CH3" s="61"/>
-      <c r="CI3" s="61"/>
-      <c r="CJ3" s="61"/>
-      <c r="CK3" s="61"/>
-      <c r="CL3" s="61"/>
-      <c r="CM3" s="61"/>
-      <c r="CN3" s="61"/>
-      <c r="CO3" s="61"/>
-      <c r="CP3" s="61"/>
-      <c r="CQ3" s="61"/>
-      <c r="CR3" s="61"/>
-      <c r="CS3" s="62"/>
-      <c r="CT3" s="60">
+      <c r="CE3" s="64"/>
+      <c r="CF3" s="64"/>
+      <c r="CG3" s="64"/>
+      <c r="CH3" s="64"/>
+      <c r="CI3" s="64"/>
+      <c r="CJ3" s="64"/>
+      <c r="CK3" s="64"/>
+      <c r="CL3" s="64"/>
+      <c r="CM3" s="64"/>
+      <c r="CN3" s="64"/>
+      <c r="CO3" s="64"/>
+      <c r="CP3" s="64"/>
+      <c r="CQ3" s="64"/>
+      <c r="CR3" s="64"/>
+      <c r="CS3" s="65"/>
+      <c r="CT3" s="63">
         <v>9</v>
       </c>
-      <c r="CU3" s="61"/>
-      <c r="CV3" s="61"/>
-      <c r="CW3" s="61"/>
-      <c r="CX3" s="61"/>
-      <c r="CY3" s="61"/>
-      <c r="CZ3" s="61"/>
-      <c r="DA3" s="61"/>
-      <c r="DB3" s="61"/>
-      <c r="DC3" s="61"/>
-      <c r="DD3" s="61"/>
-      <c r="DE3" s="61"/>
-      <c r="DF3" s="61"/>
-      <c r="DG3" s="61"/>
-      <c r="DH3" s="61"/>
-      <c r="DI3" s="62"/>
-      <c r="DJ3" s="60">
+      <c r="CU3" s="64"/>
+      <c r="CV3" s="64"/>
+      <c r="CW3" s="64"/>
+      <c r="CX3" s="64"/>
+      <c r="CY3" s="64"/>
+      <c r="CZ3" s="64"/>
+      <c r="DA3" s="64"/>
+      <c r="DB3" s="64"/>
+      <c r="DC3" s="64"/>
+      <c r="DD3" s="64"/>
+      <c r="DE3" s="64"/>
+      <c r="DF3" s="64"/>
+      <c r="DG3" s="64"/>
+      <c r="DH3" s="64"/>
+      <c r="DI3" s="65"/>
+      <c r="DJ3" s="63">
         <v>9</v>
       </c>
-      <c r="DK3" s="61"/>
-      <c r="DL3" s="61"/>
-      <c r="DM3" s="61"/>
-      <c r="DN3" s="61"/>
-      <c r="DO3" s="61"/>
-      <c r="DP3" s="61"/>
-      <c r="DQ3" s="61"/>
-      <c r="DR3" s="61"/>
-      <c r="DS3" s="61"/>
-      <c r="DT3" s="61"/>
-      <c r="DU3" s="61"/>
-      <c r="DV3" s="61"/>
-      <c r="DW3" s="61"/>
-      <c r="DX3" s="61"/>
-      <c r="DY3" s="62"/>
-      <c r="DZ3" s="63">
+      <c r="DK3" s="64"/>
+      <c r="DL3" s="64"/>
+      <c r="DM3" s="64"/>
+      <c r="DN3" s="64"/>
+      <c r="DO3" s="64"/>
+      <c r="DP3" s="64"/>
+      <c r="DQ3" s="64"/>
+      <c r="DR3" s="64"/>
+      <c r="DS3" s="64"/>
+      <c r="DT3" s="64"/>
+      <c r="DU3" s="64"/>
+      <c r="DV3" s="64"/>
+      <c r="DW3" s="64"/>
+      <c r="DX3" s="64"/>
+      <c r="DY3" s="65"/>
+      <c r="DZ3" s="66">
         <v>13</v>
       </c>
-      <c r="EA3" s="64"/>
-      <c r="EB3" s="64"/>
-      <c r="EC3" s="64"/>
-      <c r="ED3" s="64"/>
-      <c r="EE3" s="64"/>
-      <c r="EF3" s="64"/>
-      <c r="EG3" s="64"/>
-      <c r="EH3" s="64"/>
-      <c r="EI3" s="64"/>
-      <c r="EJ3" s="64"/>
-      <c r="EK3" s="64"/>
-      <c r="EL3" s="64"/>
-      <c r="EM3" s="64"/>
-      <c r="EN3" s="64"/>
-      <c r="EO3" s="65"/>
-      <c r="EP3" s="66">
+      <c r="EA3" s="61"/>
+      <c r="EB3" s="61"/>
+      <c r="EC3" s="61"/>
+      <c r="ED3" s="61"/>
+      <c r="EE3" s="61"/>
+      <c r="EF3" s="61"/>
+      <c r="EG3" s="61"/>
+      <c r="EH3" s="61"/>
+      <c r="EI3" s="61"/>
+      <c r="EJ3" s="61"/>
+      <c r="EK3" s="61"/>
+      <c r="EL3" s="61"/>
+      <c r="EM3" s="61"/>
+      <c r="EN3" s="61"/>
+      <c r="EO3" s="62"/>
+      <c r="EP3" s="60">
         <v>13</v>
       </c>
-      <c r="EQ3" s="64"/>
-      <c r="ER3" s="64"/>
-      <c r="ES3" s="64"/>
-      <c r="ET3" s="64"/>
-      <c r="EU3" s="64"/>
-      <c r="EV3" s="64"/>
-      <c r="EW3" s="64"/>
-      <c r="EX3" s="64"/>
-      <c r="EY3" s="64"/>
-      <c r="EZ3" s="64"/>
-      <c r="FA3" s="64"/>
-      <c r="FB3" s="64"/>
-      <c r="FC3" s="64"/>
-      <c r="FD3" s="64"/>
-      <c r="FE3" s="65"/>
-      <c r="FF3" s="66">
+      <c r="EQ3" s="61"/>
+      <c r="ER3" s="61"/>
+      <c r="ES3" s="61"/>
+      <c r="ET3" s="61"/>
+      <c r="EU3" s="61"/>
+      <c r="EV3" s="61"/>
+      <c r="EW3" s="61"/>
+      <c r="EX3" s="61"/>
+      <c r="EY3" s="61"/>
+      <c r="EZ3" s="61"/>
+      <c r="FA3" s="61"/>
+      <c r="FB3" s="61"/>
+      <c r="FC3" s="61"/>
+      <c r="FD3" s="61"/>
+      <c r="FE3" s="62"/>
+      <c r="FF3" s="60">
         <v>13</v>
       </c>
-      <c r="FG3" s="64"/>
-      <c r="FH3" s="64"/>
-      <c r="FI3" s="64"/>
-      <c r="FJ3" s="64"/>
-      <c r="FK3" s="64"/>
-      <c r="FL3" s="64"/>
-      <c r="FM3" s="64"/>
-      <c r="FN3" s="64"/>
-      <c r="FO3" s="64"/>
-      <c r="FP3" s="64"/>
-      <c r="FQ3" s="64"/>
-      <c r="FR3" s="64"/>
-      <c r="FS3" s="64"/>
-      <c r="FT3" s="64"/>
-      <c r="FU3" s="65"/>
-      <c r="FV3" s="66">
+      <c r="FG3" s="61"/>
+      <c r="FH3" s="61"/>
+      <c r="FI3" s="61"/>
+      <c r="FJ3" s="61"/>
+      <c r="FK3" s="61"/>
+      <c r="FL3" s="61"/>
+      <c r="FM3" s="61"/>
+      <c r="FN3" s="61"/>
+      <c r="FO3" s="61"/>
+      <c r="FP3" s="61"/>
+      <c r="FQ3" s="61"/>
+      <c r="FR3" s="61"/>
+      <c r="FS3" s="61"/>
+      <c r="FT3" s="61"/>
+      <c r="FU3" s="62"/>
+      <c r="FV3" s="60">
         <v>13</v>
       </c>
-      <c r="FW3" s="64"/>
-      <c r="FX3" s="64"/>
-      <c r="FY3" s="64"/>
-      <c r="FZ3" s="64"/>
-      <c r="GA3" s="64"/>
-      <c r="GB3" s="64"/>
-      <c r="GC3" s="64"/>
-      <c r="GD3" s="64"/>
-      <c r="GE3" s="64"/>
-      <c r="GF3" s="64"/>
-      <c r="GG3" s="64"/>
-      <c r="GH3" s="64"/>
-      <c r="GI3" s="64"/>
-      <c r="GJ3" s="64"/>
-      <c r="GK3" s="65"/>
-      <c r="GL3" s="66">
+      <c r="FW3" s="61"/>
+      <c r="FX3" s="61"/>
+      <c r="FY3" s="61"/>
+      <c r="FZ3" s="61"/>
+      <c r="GA3" s="61"/>
+      <c r="GB3" s="61"/>
+      <c r="GC3" s="61"/>
+      <c r="GD3" s="61"/>
+      <c r="GE3" s="61"/>
+      <c r="GF3" s="61"/>
+      <c r="GG3" s="61"/>
+      <c r="GH3" s="61"/>
+      <c r="GI3" s="61"/>
+      <c r="GJ3" s="61"/>
+      <c r="GK3" s="62"/>
+      <c r="GL3" s="60">
         <v>17</v>
       </c>
-      <c r="GM3" s="64"/>
-      <c r="GN3" s="64"/>
-      <c r="GO3" s="64"/>
-      <c r="GP3" s="64"/>
-      <c r="GQ3" s="64"/>
-      <c r="GR3" s="64"/>
-      <c r="GS3" s="64"/>
-      <c r="GT3" s="64"/>
-      <c r="GU3" s="64"/>
-      <c r="GV3" s="64"/>
-      <c r="GW3" s="64"/>
-      <c r="GX3" s="64"/>
-      <c r="GY3" s="64"/>
-      <c r="GZ3" s="64"/>
-      <c r="HA3" s="65"/>
-      <c r="HB3" s="66">
+      <c r="GM3" s="61"/>
+      <c r="GN3" s="61"/>
+      <c r="GO3" s="61"/>
+      <c r="GP3" s="61"/>
+      <c r="GQ3" s="61"/>
+      <c r="GR3" s="61"/>
+      <c r="GS3" s="61"/>
+      <c r="GT3" s="61"/>
+      <c r="GU3" s="61"/>
+      <c r="GV3" s="61"/>
+      <c r="GW3" s="61"/>
+      <c r="GX3" s="61"/>
+      <c r="GY3" s="61"/>
+      <c r="GZ3" s="61"/>
+      <c r="HA3" s="62"/>
+      <c r="HB3" s="60">
         <v>17</v>
       </c>
-      <c r="HC3" s="64"/>
-      <c r="HD3" s="64"/>
-      <c r="HE3" s="64"/>
-      <c r="HF3" s="64"/>
-      <c r="HG3" s="64"/>
-      <c r="HH3" s="64"/>
-      <c r="HI3" s="64"/>
-      <c r="HJ3" s="64"/>
-      <c r="HK3" s="64"/>
-      <c r="HL3" s="64"/>
-      <c r="HM3" s="64"/>
-      <c r="HN3" s="64"/>
-      <c r="HO3" s="64"/>
-      <c r="HP3" s="64"/>
-      <c r="HQ3" s="65"/>
-      <c r="HR3" s="66">
+      <c r="HC3" s="61"/>
+      <c r="HD3" s="61"/>
+      <c r="HE3" s="61"/>
+      <c r="HF3" s="61"/>
+      <c r="HG3" s="61"/>
+      <c r="HH3" s="61"/>
+      <c r="HI3" s="61"/>
+      <c r="HJ3" s="61"/>
+      <c r="HK3" s="61"/>
+      <c r="HL3" s="61"/>
+      <c r="HM3" s="61"/>
+      <c r="HN3" s="61"/>
+      <c r="HO3" s="61"/>
+      <c r="HP3" s="61"/>
+      <c r="HQ3" s="62"/>
+      <c r="HR3" s="60">
         <v>17</v>
       </c>
-      <c r="HS3" s="64"/>
-      <c r="HT3" s="64"/>
-      <c r="HU3" s="64"/>
-      <c r="HV3" s="64"/>
-      <c r="HW3" s="64"/>
-      <c r="HX3" s="64"/>
-      <c r="HY3" s="64"/>
-      <c r="HZ3" s="64"/>
-      <c r="IA3" s="64"/>
-      <c r="IB3" s="64"/>
-      <c r="IC3" s="64"/>
-      <c r="ID3" s="64"/>
-      <c r="IE3" s="64"/>
-      <c r="IF3" s="64"/>
-      <c r="IG3" s="65"/>
-      <c r="IH3" s="66">
+      <c r="HS3" s="61"/>
+      <c r="HT3" s="61"/>
+      <c r="HU3" s="61"/>
+      <c r="HV3" s="61"/>
+      <c r="HW3" s="61"/>
+      <c r="HX3" s="61"/>
+      <c r="HY3" s="61"/>
+      <c r="HZ3" s="61"/>
+      <c r="IA3" s="61"/>
+      <c r="IB3" s="61"/>
+      <c r="IC3" s="61"/>
+      <c r="ID3" s="61"/>
+      <c r="IE3" s="61"/>
+      <c r="IF3" s="61"/>
+      <c r="IG3" s="62"/>
+      <c r="IH3" s="60">
         <v>17</v>
       </c>
-      <c r="II3" s="64"/>
-      <c r="IJ3" s="64"/>
-      <c r="IK3" s="64"/>
-      <c r="IL3" s="64"/>
-      <c r="IM3" s="64"/>
-      <c r="IN3" s="64"/>
-      <c r="IO3" s="64"/>
-      <c r="IP3" s="64"/>
-      <c r="IQ3" s="64"/>
-      <c r="IR3" s="64"/>
-      <c r="IS3" s="64"/>
-      <c r="IT3" s="64"/>
-      <c r="IU3" s="64"/>
-      <c r="IV3" s="64"/>
-      <c r="IW3" s="65"/>
+      <c r="II3" s="61"/>
+      <c r="IJ3" s="61"/>
+      <c r="IK3" s="61"/>
+      <c r="IL3" s="61"/>
+      <c r="IM3" s="61"/>
+      <c r="IN3" s="61"/>
+      <c r="IO3" s="61"/>
+      <c r="IP3" s="61"/>
+      <c r="IQ3" s="61"/>
+      <c r="IR3" s="61"/>
+      <c r="IS3" s="61"/>
+      <c r="IT3" s="61"/>
+      <c r="IU3" s="61"/>
+      <c r="IV3" s="61"/>
+      <c r="IW3" s="62"/>
     </row>
     <row r="4" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -29977,19 +30012,57 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="HB2:HQ2"/>
-    <mergeCell ref="HR2:IG2"/>
-    <mergeCell ref="IH2:IW2"/>
-    <mergeCell ref="DZ2:EO2"/>
-    <mergeCell ref="EP2:FE2"/>
-    <mergeCell ref="FF2:FU2"/>
-    <mergeCell ref="FV2:GK2"/>
-    <mergeCell ref="GL2:HA2"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="BN2:CC2"/>
-    <mergeCell ref="CD2:CS2"/>
-    <mergeCell ref="CT2:DI2"/>
-    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AH4:AO4"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="BN4:BU4"/>
+    <mergeCell ref="BV4:CC4"/>
+    <mergeCell ref="CD4:CK4"/>
+    <mergeCell ref="CL4:CS4"/>
+    <mergeCell ref="CT4:DA4"/>
+    <mergeCell ref="DB4:DI4"/>
+    <mergeCell ref="DJ4:DQ4"/>
+    <mergeCell ref="DR4:DY4"/>
+    <mergeCell ref="DZ4:EG4"/>
+    <mergeCell ref="EH4:EO4"/>
+    <mergeCell ref="EP4:EW4"/>
+    <mergeCell ref="EX4:FE4"/>
+    <mergeCell ref="FF4:FM4"/>
+    <mergeCell ref="FN4:FU4"/>
+    <mergeCell ref="FV4:GC4"/>
+    <mergeCell ref="GD4:GK4"/>
+    <mergeCell ref="GL4:GS4"/>
+    <mergeCell ref="GT4:HA4"/>
+    <mergeCell ref="HB4:HI4"/>
+    <mergeCell ref="HJ4:HQ4"/>
+    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="HZ4:IG4"/>
+    <mergeCell ref="IH4:IO4"/>
+    <mergeCell ref="IP4:IW4"/>
+    <mergeCell ref="AH3:AW3"/>
+    <mergeCell ref="AX3:BM3"/>
+    <mergeCell ref="BN3:CC3"/>
+    <mergeCell ref="CD3:CS3"/>
+    <mergeCell ref="CT3:DI3"/>
+    <mergeCell ref="DJ3:DY3"/>
+    <mergeCell ref="DZ3:EO3"/>
+    <mergeCell ref="EP3:FE3"/>
+    <mergeCell ref="FF3:FU3"/>
+    <mergeCell ref="FV3:GK3"/>
+    <mergeCell ref="GL3:HA3"/>
+    <mergeCell ref="HB3:HQ3"/>
+    <mergeCell ref="HR3:IG3"/>
     <mergeCell ref="IH3:IW3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AX1:BM1"/>
@@ -30006,57 +30079,19 @@
     <mergeCell ref="HR1:IG1"/>
     <mergeCell ref="IH1:IW1"/>
     <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="HZ4:IG4"/>
-    <mergeCell ref="IH4:IO4"/>
-    <mergeCell ref="IP4:IW4"/>
-    <mergeCell ref="AH3:AW3"/>
-    <mergeCell ref="AX3:BM3"/>
-    <mergeCell ref="BN3:CC3"/>
-    <mergeCell ref="CD3:CS3"/>
-    <mergeCell ref="CT3:DI3"/>
-    <mergeCell ref="DJ3:DY3"/>
-    <mergeCell ref="DZ3:EO3"/>
-    <mergeCell ref="EP3:FE3"/>
-    <mergeCell ref="FF3:FU3"/>
-    <mergeCell ref="FV3:GK3"/>
-    <mergeCell ref="GL3:HA3"/>
-    <mergeCell ref="HB3:HQ3"/>
-    <mergeCell ref="HR3:IG3"/>
-    <mergeCell ref="GL4:GS4"/>
-    <mergeCell ref="GT4:HA4"/>
-    <mergeCell ref="HB4:HI4"/>
-    <mergeCell ref="HJ4:HQ4"/>
-    <mergeCell ref="HR4:HY4"/>
-    <mergeCell ref="EX4:FE4"/>
-    <mergeCell ref="FF4:FM4"/>
-    <mergeCell ref="FN4:FU4"/>
-    <mergeCell ref="FV4:GC4"/>
-    <mergeCell ref="GD4:GK4"/>
-    <mergeCell ref="DJ4:DQ4"/>
-    <mergeCell ref="DR4:DY4"/>
-    <mergeCell ref="DZ4:EG4"/>
-    <mergeCell ref="EH4:EO4"/>
-    <mergeCell ref="EP4:EW4"/>
-    <mergeCell ref="BV4:CC4"/>
-    <mergeCell ref="CD4:CK4"/>
-    <mergeCell ref="CL4:CS4"/>
-    <mergeCell ref="CT4:DA4"/>
-    <mergeCell ref="DB4:DI4"/>
-    <mergeCell ref="AH4:AO4"/>
-    <mergeCell ref="AP4:AW4"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="BF4:BM4"/>
-    <mergeCell ref="BN4:BU4"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="BN2:CC2"/>
+    <mergeCell ref="CD2:CS2"/>
+    <mergeCell ref="CT2:DI2"/>
+    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="HB2:HQ2"/>
+    <mergeCell ref="HR2:IG2"/>
+    <mergeCell ref="IH2:IW2"/>
+    <mergeCell ref="DZ2:EO2"/>
+    <mergeCell ref="EP2:FE2"/>
+    <mergeCell ref="FF2:FU2"/>
+    <mergeCell ref="FV2:GK2"/>
+    <mergeCell ref="GL2:HA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Jupyter notebook analysis added
</commit_message>
<xml_diff>
--- a/Data/OurData2.xlsx
+++ b/Data/OurData2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CD28D3-87F6-F74D-AA19-039383E25C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E819DE44-AA17-3D47-82C3-E6AB1767FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="500" windowWidth="28800" windowHeight="16060" firstSheet="1" activeTab="11" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
@@ -1587,15 +1587,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1606,6 +1597,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5745,7 +5745,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5780,7 +5780,7 @@
         <v>120</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>127</v>
+        <v>334</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>121</v>
@@ -18367,6 +18367,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AH1:AW1"/>
+    <mergeCell ref="AH2:AW2"/>
+    <mergeCell ref="AH3:AO3"/>
+    <mergeCell ref="AP3:AW3"/>
+    <mergeCell ref="AX1:BM1"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="AX3:BE3"/>
+    <mergeCell ref="BF3:BM3"/>
     <mergeCell ref="B3:I3"/>
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="B1:Q1"/>
@@ -18375,14 +18383,6 @@
     <mergeCell ref="R2:AG2"/>
     <mergeCell ref="R3:Y3"/>
     <mergeCell ref="Z3:AG3"/>
-    <mergeCell ref="AH1:AW1"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="AH3:AO3"/>
-    <mergeCell ref="AP3:AW3"/>
-    <mergeCell ref="AX1:BM1"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="AX3:BE3"/>
-    <mergeCell ref="BF3:BM3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19024,294 +19024,294 @@
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="63">
-        <v>5</v>
-      </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="63">
-        <v>5</v>
-      </c>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="65"/>
-      <c r="AH3" s="63">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="64"/>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
-      <c r="AW3" s="65"/>
-      <c r="AX3" s="63">
-        <v>5</v>
-      </c>
-      <c r="AY3" s="64"/>
-      <c r="AZ3" s="64"/>
-      <c r="BA3" s="64"/>
-      <c r="BB3" s="64"/>
-      <c r="BC3" s="64"/>
-      <c r="BD3" s="64"/>
-      <c r="BE3" s="64"/>
-      <c r="BF3" s="64"/>
-      <c r="BG3" s="64"/>
-      <c r="BH3" s="64"/>
-      <c r="BI3" s="64"/>
-      <c r="BJ3" s="64"/>
-      <c r="BK3" s="64"/>
-      <c r="BL3" s="64"/>
-      <c r="BM3" s="65"/>
-      <c r="BN3" s="63">
+      <c r="B3" s="60">
+        <v>5</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="60">
+        <v>5</v>
+      </c>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="61"/>
+      <c r="AB3" s="61"/>
+      <c r="AC3" s="61"/>
+      <c r="AD3" s="61"/>
+      <c r="AE3" s="61"/>
+      <c r="AF3" s="61"/>
+      <c r="AG3" s="62"/>
+      <c r="AH3" s="60">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="61"/>
+      <c r="AJ3" s="61"/>
+      <c r="AK3" s="61"/>
+      <c r="AL3" s="61"/>
+      <c r="AM3" s="61"/>
+      <c r="AN3" s="61"/>
+      <c r="AO3" s="61"/>
+      <c r="AP3" s="61"/>
+      <c r="AQ3" s="61"/>
+      <c r="AR3" s="61"/>
+      <c r="AS3" s="61"/>
+      <c r="AT3" s="61"/>
+      <c r="AU3" s="61"/>
+      <c r="AV3" s="61"/>
+      <c r="AW3" s="62"/>
+      <c r="AX3" s="60">
+        <v>5</v>
+      </c>
+      <c r="AY3" s="61"/>
+      <c r="AZ3" s="61"/>
+      <c r="BA3" s="61"/>
+      <c r="BB3" s="61"/>
+      <c r="BC3" s="61"/>
+      <c r="BD3" s="61"/>
+      <c r="BE3" s="61"/>
+      <c r="BF3" s="61"/>
+      <c r="BG3" s="61"/>
+      <c r="BH3" s="61"/>
+      <c r="BI3" s="61"/>
+      <c r="BJ3" s="61"/>
+      <c r="BK3" s="61"/>
+      <c r="BL3" s="61"/>
+      <c r="BM3" s="62"/>
+      <c r="BN3" s="60">
         <v>9</v>
       </c>
-      <c r="BO3" s="64"/>
-      <c r="BP3" s="64"/>
-      <c r="BQ3" s="64"/>
-      <c r="BR3" s="64"/>
-      <c r="BS3" s="64"/>
-      <c r="BT3" s="64"/>
-      <c r="BU3" s="64"/>
-      <c r="BV3" s="64"/>
-      <c r="BW3" s="64"/>
-      <c r="BX3" s="64"/>
-      <c r="BY3" s="64"/>
-      <c r="BZ3" s="64"/>
-      <c r="CA3" s="64"/>
-      <c r="CB3" s="64"/>
-      <c r="CC3" s="65"/>
-      <c r="CD3" s="63">
+      <c r="BO3" s="61"/>
+      <c r="BP3" s="61"/>
+      <c r="BQ3" s="61"/>
+      <c r="BR3" s="61"/>
+      <c r="BS3" s="61"/>
+      <c r="BT3" s="61"/>
+      <c r="BU3" s="61"/>
+      <c r="BV3" s="61"/>
+      <c r="BW3" s="61"/>
+      <c r="BX3" s="61"/>
+      <c r="BY3" s="61"/>
+      <c r="BZ3" s="61"/>
+      <c r="CA3" s="61"/>
+      <c r="CB3" s="61"/>
+      <c r="CC3" s="62"/>
+      <c r="CD3" s="60">
         <v>9</v>
       </c>
-      <c r="CE3" s="64"/>
-      <c r="CF3" s="64"/>
-      <c r="CG3" s="64"/>
-      <c r="CH3" s="64"/>
-      <c r="CI3" s="64"/>
-      <c r="CJ3" s="64"/>
-      <c r="CK3" s="64"/>
-      <c r="CL3" s="64"/>
-      <c r="CM3" s="64"/>
-      <c r="CN3" s="64"/>
-      <c r="CO3" s="64"/>
-      <c r="CP3" s="64"/>
-      <c r="CQ3" s="64"/>
-      <c r="CR3" s="64"/>
-      <c r="CS3" s="65"/>
-      <c r="CT3" s="63">
+      <c r="CE3" s="61"/>
+      <c r="CF3" s="61"/>
+      <c r="CG3" s="61"/>
+      <c r="CH3" s="61"/>
+      <c r="CI3" s="61"/>
+      <c r="CJ3" s="61"/>
+      <c r="CK3" s="61"/>
+      <c r="CL3" s="61"/>
+      <c r="CM3" s="61"/>
+      <c r="CN3" s="61"/>
+      <c r="CO3" s="61"/>
+      <c r="CP3" s="61"/>
+      <c r="CQ3" s="61"/>
+      <c r="CR3" s="61"/>
+      <c r="CS3" s="62"/>
+      <c r="CT3" s="60">
         <v>9</v>
       </c>
-      <c r="CU3" s="64"/>
-      <c r="CV3" s="64"/>
-      <c r="CW3" s="64"/>
-      <c r="CX3" s="64"/>
-      <c r="CY3" s="64"/>
-      <c r="CZ3" s="64"/>
-      <c r="DA3" s="64"/>
-      <c r="DB3" s="64"/>
-      <c r="DC3" s="64"/>
-      <c r="DD3" s="64"/>
-      <c r="DE3" s="64"/>
-      <c r="DF3" s="64"/>
-      <c r="DG3" s="64"/>
-      <c r="DH3" s="64"/>
-      <c r="DI3" s="65"/>
-      <c r="DJ3" s="63">
+      <c r="CU3" s="61"/>
+      <c r="CV3" s="61"/>
+      <c r="CW3" s="61"/>
+      <c r="CX3" s="61"/>
+      <c r="CY3" s="61"/>
+      <c r="CZ3" s="61"/>
+      <c r="DA3" s="61"/>
+      <c r="DB3" s="61"/>
+      <c r="DC3" s="61"/>
+      <c r="DD3" s="61"/>
+      <c r="DE3" s="61"/>
+      <c r="DF3" s="61"/>
+      <c r="DG3" s="61"/>
+      <c r="DH3" s="61"/>
+      <c r="DI3" s="62"/>
+      <c r="DJ3" s="60">
         <v>9</v>
       </c>
-      <c r="DK3" s="64"/>
-      <c r="DL3" s="64"/>
-      <c r="DM3" s="64"/>
-      <c r="DN3" s="64"/>
-      <c r="DO3" s="64"/>
-      <c r="DP3" s="64"/>
-      <c r="DQ3" s="64"/>
-      <c r="DR3" s="64"/>
-      <c r="DS3" s="64"/>
-      <c r="DT3" s="64"/>
-      <c r="DU3" s="64"/>
-      <c r="DV3" s="64"/>
-      <c r="DW3" s="64"/>
-      <c r="DX3" s="64"/>
-      <c r="DY3" s="65"/>
-      <c r="DZ3" s="66">
+      <c r="DK3" s="61"/>
+      <c r="DL3" s="61"/>
+      <c r="DM3" s="61"/>
+      <c r="DN3" s="61"/>
+      <c r="DO3" s="61"/>
+      <c r="DP3" s="61"/>
+      <c r="DQ3" s="61"/>
+      <c r="DR3" s="61"/>
+      <c r="DS3" s="61"/>
+      <c r="DT3" s="61"/>
+      <c r="DU3" s="61"/>
+      <c r="DV3" s="61"/>
+      <c r="DW3" s="61"/>
+      <c r="DX3" s="61"/>
+      <c r="DY3" s="62"/>
+      <c r="DZ3" s="63">
         <v>13</v>
       </c>
-      <c r="EA3" s="61"/>
-      <c r="EB3" s="61"/>
-      <c r="EC3" s="61"/>
-      <c r="ED3" s="61"/>
-      <c r="EE3" s="61"/>
-      <c r="EF3" s="61"/>
-      <c r="EG3" s="61"/>
-      <c r="EH3" s="61"/>
-      <c r="EI3" s="61"/>
-      <c r="EJ3" s="61"/>
-      <c r="EK3" s="61"/>
-      <c r="EL3" s="61"/>
-      <c r="EM3" s="61"/>
-      <c r="EN3" s="61"/>
-      <c r="EO3" s="62"/>
-      <c r="EP3" s="60">
+      <c r="EA3" s="64"/>
+      <c r="EB3" s="64"/>
+      <c r="EC3" s="64"/>
+      <c r="ED3" s="64"/>
+      <c r="EE3" s="64"/>
+      <c r="EF3" s="64"/>
+      <c r="EG3" s="64"/>
+      <c r="EH3" s="64"/>
+      <c r="EI3" s="64"/>
+      <c r="EJ3" s="64"/>
+      <c r="EK3" s="64"/>
+      <c r="EL3" s="64"/>
+      <c r="EM3" s="64"/>
+      <c r="EN3" s="64"/>
+      <c r="EO3" s="65"/>
+      <c r="EP3" s="66">
         <v>13</v>
       </c>
-      <c r="EQ3" s="61"/>
-      <c r="ER3" s="61"/>
-      <c r="ES3" s="61"/>
-      <c r="ET3" s="61"/>
-      <c r="EU3" s="61"/>
-      <c r="EV3" s="61"/>
-      <c r="EW3" s="61"/>
-      <c r="EX3" s="61"/>
-      <c r="EY3" s="61"/>
-      <c r="EZ3" s="61"/>
-      <c r="FA3" s="61"/>
-      <c r="FB3" s="61"/>
-      <c r="FC3" s="61"/>
-      <c r="FD3" s="61"/>
-      <c r="FE3" s="62"/>
-      <c r="FF3" s="60">
+      <c r="EQ3" s="64"/>
+      <c r="ER3" s="64"/>
+      <c r="ES3" s="64"/>
+      <c r="ET3" s="64"/>
+      <c r="EU3" s="64"/>
+      <c r="EV3" s="64"/>
+      <c r="EW3" s="64"/>
+      <c r="EX3" s="64"/>
+      <c r="EY3" s="64"/>
+      <c r="EZ3" s="64"/>
+      <c r="FA3" s="64"/>
+      <c r="FB3" s="64"/>
+      <c r="FC3" s="64"/>
+      <c r="FD3" s="64"/>
+      <c r="FE3" s="65"/>
+      <c r="FF3" s="66">
         <v>13</v>
       </c>
-      <c r="FG3" s="61"/>
-      <c r="FH3" s="61"/>
-      <c r="FI3" s="61"/>
-      <c r="FJ3" s="61"/>
-      <c r="FK3" s="61"/>
-      <c r="FL3" s="61"/>
-      <c r="FM3" s="61"/>
-      <c r="FN3" s="61"/>
-      <c r="FO3" s="61"/>
-      <c r="FP3" s="61"/>
-      <c r="FQ3" s="61"/>
-      <c r="FR3" s="61"/>
-      <c r="FS3" s="61"/>
-      <c r="FT3" s="61"/>
-      <c r="FU3" s="62"/>
-      <c r="FV3" s="60">
+      <c r="FG3" s="64"/>
+      <c r="FH3" s="64"/>
+      <c r="FI3" s="64"/>
+      <c r="FJ3" s="64"/>
+      <c r="FK3" s="64"/>
+      <c r="FL3" s="64"/>
+      <c r="FM3" s="64"/>
+      <c r="FN3" s="64"/>
+      <c r="FO3" s="64"/>
+      <c r="FP3" s="64"/>
+      <c r="FQ3" s="64"/>
+      <c r="FR3" s="64"/>
+      <c r="FS3" s="64"/>
+      <c r="FT3" s="64"/>
+      <c r="FU3" s="65"/>
+      <c r="FV3" s="66">
         <v>13</v>
       </c>
-      <c r="FW3" s="61"/>
-      <c r="FX3" s="61"/>
-      <c r="FY3" s="61"/>
-      <c r="FZ3" s="61"/>
-      <c r="GA3" s="61"/>
-      <c r="GB3" s="61"/>
-      <c r="GC3" s="61"/>
-      <c r="GD3" s="61"/>
-      <c r="GE3" s="61"/>
-      <c r="GF3" s="61"/>
-      <c r="GG3" s="61"/>
-      <c r="GH3" s="61"/>
-      <c r="GI3" s="61"/>
-      <c r="GJ3" s="61"/>
-      <c r="GK3" s="62"/>
-      <c r="GL3" s="60">
+      <c r="FW3" s="64"/>
+      <c r="FX3" s="64"/>
+      <c r="FY3" s="64"/>
+      <c r="FZ3" s="64"/>
+      <c r="GA3" s="64"/>
+      <c r="GB3" s="64"/>
+      <c r="GC3" s="64"/>
+      <c r="GD3" s="64"/>
+      <c r="GE3" s="64"/>
+      <c r="GF3" s="64"/>
+      <c r="GG3" s="64"/>
+      <c r="GH3" s="64"/>
+      <c r="GI3" s="64"/>
+      <c r="GJ3" s="64"/>
+      <c r="GK3" s="65"/>
+      <c r="GL3" s="66">
         <v>17</v>
       </c>
-      <c r="GM3" s="61"/>
-      <c r="GN3" s="61"/>
-      <c r="GO3" s="61"/>
-      <c r="GP3" s="61"/>
-      <c r="GQ3" s="61"/>
-      <c r="GR3" s="61"/>
-      <c r="GS3" s="61"/>
-      <c r="GT3" s="61"/>
-      <c r="GU3" s="61"/>
-      <c r="GV3" s="61"/>
-      <c r="GW3" s="61"/>
-      <c r="GX3" s="61"/>
-      <c r="GY3" s="61"/>
-      <c r="GZ3" s="61"/>
-      <c r="HA3" s="62"/>
-      <c r="HB3" s="60">
+      <c r="GM3" s="64"/>
+      <c r="GN3" s="64"/>
+      <c r="GO3" s="64"/>
+      <c r="GP3" s="64"/>
+      <c r="GQ3" s="64"/>
+      <c r="GR3" s="64"/>
+      <c r="GS3" s="64"/>
+      <c r="GT3" s="64"/>
+      <c r="GU3" s="64"/>
+      <c r="GV3" s="64"/>
+      <c r="GW3" s="64"/>
+      <c r="GX3" s="64"/>
+      <c r="GY3" s="64"/>
+      <c r="GZ3" s="64"/>
+      <c r="HA3" s="65"/>
+      <c r="HB3" s="66">
         <v>17</v>
       </c>
-      <c r="HC3" s="61"/>
-      <c r="HD3" s="61"/>
-      <c r="HE3" s="61"/>
-      <c r="HF3" s="61"/>
-      <c r="HG3" s="61"/>
-      <c r="HH3" s="61"/>
-      <c r="HI3" s="61"/>
-      <c r="HJ3" s="61"/>
-      <c r="HK3" s="61"/>
-      <c r="HL3" s="61"/>
-      <c r="HM3" s="61"/>
-      <c r="HN3" s="61"/>
-      <c r="HO3" s="61"/>
-      <c r="HP3" s="61"/>
-      <c r="HQ3" s="62"/>
-      <c r="HR3" s="60">
+      <c r="HC3" s="64"/>
+      <c r="HD3" s="64"/>
+      <c r="HE3" s="64"/>
+      <c r="HF3" s="64"/>
+      <c r="HG3" s="64"/>
+      <c r="HH3" s="64"/>
+      <c r="HI3" s="64"/>
+      <c r="HJ3" s="64"/>
+      <c r="HK3" s="64"/>
+      <c r="HL3" s="64"/>
+      <c r="HM3" s="64"/>
+      <c r="HN3" s="64"/>
+      <c r="HO3" s="64"/>
+      <c r="HP3" s="64"/>
+      <c r="HQ3" s="65"/>
+      <c r="HR3" s="66">
         <v>17</v>
       </c>
-      <c r="HS3" s="61"/>
-      <c r="HT3" s="61"/>
-      <c r="HU3" s="61"/>
-      <c r="HV3" s="61"/>
-      <c r="HW3" s="61"/>
-      <c r="HX3" s="61"/>
-      <c r="HY3" s="61"/>
-      <c r="HZ3" s="61"/>
-      <c r="IA3" s="61"/>
-      <c r="IB3" s="61"/>
-      <c r="IC3" s="61"/>
-      <c r="ID3" s="61"/>
-      <c r="IE3" s="61"/>
-      <c r="IF3" s="61"/>
-      <c r="IG3" s="62"/>
-      <c r="IH3" s="60">
+      <c r="HS3" s="64"/>
+      <c r="HT3" s="64"/>
+      <c r="HU3" s="64"/>
+      <c r="HV3" s="64"/>
+      <c r="HW3" s="64"/>
+      <c r="HX3" s="64"/>
+      <c r="HY3" s="64"/>
+      <c r="HZ3" s="64"/>
+      <c r="IA3" s="64"/>
+      <c r="IB3" s="64"/>
+      <c r="IC3" s="64"/>
+      <c r="ID3" s="64"/>
+      <c r="IE3" s="64"/>
+      <c r="IF3" s="64"/>
+      <c r="IG3" s="65"/>
+      <c r="IH3" s="66">
         <v>17</v>
       </c>
-      <c r="II3" s="61"/>
-      <c r="IJ3" s="61"/>
-      <c r="IK3" s="61"/>
-      <c r="IL3" s="61"/>
-      <c r="IM3" s="61"/>
-      <c r="IN3" s="61"/>
-      <c r="IO3" s="61"/>
-      <c r="IP3" s="61"/>
-      <c r="IQ3" s="61"/>
-      <c r="IR3" s="61"/>
-      <c r="IS3" s="61"/>
-      <c r="IT3" s="61"/>
-      <c r="IU3" s="61"/>
-      <c r="IV3" s="61"/>
-      <c r="IW3" s="62"/>
+      <c r="II3" s="64"/>
+      <c r="IJ3" s="64"/>
+      <c r="IK3" s="64"/>
+      <c r="IL3" s="64"/>
+      <c r="IM3" s="64"/>
+      <c r="IN3" s="64"/>
+      <c r="IO3" s="64"/>
+      <c r="IP3" s="64"/>
+      <c r="IQ3" s="64"/>
+      <c r="IR3" s="64"/>
+      <c r="IS3" s="64"/>
+      <c r="IT3" s="64"/>
+      <c r="IU3" s="64"/>
+      <c r="IV3" s="64"/>
+      <c r="IW3" s="65"/>
     </row>
     <row r="4" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -30012,41 +30012,35 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="R3:AG3"/>
-    <mergeCell ref="AH4:AO4"/>
-    <mergeCell ref="AP4:AW4"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="BF4:BM4"/>
-    <mergeCell ref="BN4:BU4"/>
-    <mergeCell ref="BV4:CC4"/>
-    <mergeCell ref="CD4:CK4"/>
-    <mergeCell ref="CL4:CS4"/>
-    <mergeCell ref="CT4:DA4"/>
-    <mergeCell ref="DB4:DI4"/>
-    <mergeCell ref="DJ4:DQ4"/>
-    <mergeCell ref="DR4:DY4"/>
-    <mergeCell ref="DZ4:EG4"/>
-    <mergeCell ref="EH4:EO4"/>
-    <mergeCell ref="EP4:EW4"/>
-    <mergeCell ref="EX4:FE4"/>
-    <mergeCell ref="FF4:FM4"/>
-    <mergeCell ref="FN4:FU4"/>
-    <mergeCell ref="FV4:GC4"/>
-    <mergeCell ref="GD4:GK4"/>
-    <mergeCell ref="GL4:GS4"/>
-    <mergeCell ref="GT4:HA4"/>
-    <mergeCell ref="HB4:HI4"/>
-    <mergeCell ref="HJ4:HQ4"/>
-    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="HB2:HQ2"/>
+    <mergeCell ref="HR2:IG2"/>
+    <mergeCell ref="IH2:IW2"/>
+    <mergeCell ref="DZ2:EO2"/>
+    <mergeCell ref="EP2:FE2"/>
+    <mergeCell ref="FF2:FU2"/>
+    <mergeCell ref="FV2:GK2"/>
+    <mergeCell ref="GL2:HA2"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="BN2:CC2"/>
+    <mergeCell ref="CD2:CS2"/>
+    <mergeCell ref="CT2:DI2"/>
+    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="IH3:IW3"/>
+    <mergeCell ref="AH1:AW1"/>
+    <mergeCell ref="AX1:BM1"/>
+    <mergeCell ref="BN1:CC1"/>
+    <mergeCell ref="CD1:CS1"/>
+    <mergeCell ref="CT1:DI1"/>
+    <mergeCell ref="DJ1:DY1"/>
+    <mergeCell ref="DZ1:EO1"/>
+    <mergeCell ref="EP1:FE1"/>
+    <mergeCell ref="FF1:FU1"/>
+    <mergeCell ref="FV1:GK1"/>
+    <mergeCell ref="GL1:HA1"/>
+    <mergeCell ref="HB1:HQ1"/>
+    <mergeCell ref="HR1:IG1"/>
+    <mergeCell ref="IH1:IW1"/>
+    <mergeCell ref="AH2:AW2"/>
     <mergeCell ref="HZ4:IG4"/>
     <mergeCell ref="IH4:IO4"/>
     <mergeCell ref="IP4:IW4"/>
@@ -30063,35 +30057,41 @@
     <mergeCell ref="GL3:HA3"/>
     <mergeCell ref="HB3:HQ3"/>
     <mergeCell ref="HR3:IG3"/>
-    <mergeCell ref="IH3:IW3"/>
-    <mergeCell ref="AH1:AW1"/>
-    <mergeCell ref="AX1:BM1"/>
-    <mergeCell ref="BN1:CC1"/>
-    <mergeCell ref="CD1:CS1"/>
-    <mergeCell ref="CT1:DI1"/>
-    <mergeCell ref="DJ1:DY1"/>
-    <mergeCell ref="DZ1:EO1"/>
-    <mergeCell ref="EP1:FE1"/>
-    <mergeCell ref="FF1:FU1"/>
-    <mergeCell ref="FV1:GK1"/>
-    <mergeCell ref="GL1:HA1"/>
-    <mergeCell ref="HB1:HQ1"/>
-    <mergeCell ref="HR1:IG1"/>
-    <mergeCell ref="IH1:IW1"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="BN2:CC2"/>
-    <mergeCell ref="CD2:CS2"/>
-    <mergeCell ref="CT2:DI2"/>
-    <mergeCell ref="DJ2:DY2"/>
-    <mergeCell ref="HB2:HQ2"/>
-    <mergeCell ref="HR2:IG2"/>
-    <mergeCell ref="IH2:IW2"/>
-    <mergeCell ref="DZ2:EO2"/>
-    <mergeCell ref="EP2:FE2"/>
-    <mergeCell ref="FF2:FU2"/>
-    <mergeCell ref="FV2:GK2"/>
-    <mergeCell ref="GL2:HA2"/>
+    <mergeCell ref="GL4:GS4"/>
+    <mergeCell ref="GT4:HA4"/>
+    <mergeCell ref="HB4:HI4"/>
+    <mergeCell ref="HJ4:HQ4"/>
+    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="EX4:FE4"/>
+    <mergeCell ref="FF4:FM4"/>
+    <mergeCell ref="FN4:FU4"/>
+    <mergeCell ref="FV4:GC4"/>
+    <mergeCell ref="GD4:GK4"/>
+    <mergeCell ref="DJ4:DQ4"/>
+    <mergeCell ref="DR4:DY4"/>
+    <mergeCell ref="DZ4:EG4"/>
+    <mergeCell ref="EH4:EO4"/>
+    <mergeCell ref="EP4:EW4"/>
+    <mergeCell ref="BV4:CC4"/>
+    <mergeCell ref="CD4:CK4"/>
+    <mergeCell ref="CL4:CS4"/>
+    <mergeCell ref="CT4:DA4"/>
+    <mergeCell ref="DB4:DI4"/>
+    <mergeCell ref="AH4:AO4"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="BN4:BU4"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="R3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New way of storing solution
</commit_message>
<xml_diff>
--- a/Data/OurData2.xlsx
+++ b/Data/OurData2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E819DE44-AA17-3D47-82C3-E6AB1767FD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC10037-0E9C-DB4B-A0B6-C54C2E3C291D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="500" windowWidth="28800" windowHeight="16060" firstSheet="1" activeTab="11" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
@@ -1587,6 +1587,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1597,15 +1606,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5745,7 +5745,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B9" sqref="B9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5815,7 +5815,7 @@
         <v>0.2</v>
       </c>
       <c r="F2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0.2</v>
@@ -5832,7 +5832,7 @@
       </c>
       <c r="L2" cm="1">
         <f t="array" ref="L2">SUM(B2:I2*MAX('Demand Stage 1'!$B$5:$I$8))</f>
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -5926,7 +5926,7 @@
         <v>0.75</v>
       </c>
       <c r="F5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0.75</v>
@@ -5943,7 +5943,7 @@
       </c>
       <c r="L5" cm="1">
         <f t="array" ref="L5">SUM(B5:I5*MAX('Demand Stage 1'!$B$5:$I$8))</f>
-        <v>292.5</v>
+        <v>258.75</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -6117,7 +6117,7 @@
       </c>
       <c r="F10">
         <f>SUM(F2:F9)</f>
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -6133,7 +6133,7 @@
       </c>
       <c r="L10" cm="1">
         <f t="array" ref="L10">SUM(B10:I10*MAX('Demand Stage 1'!$B$5:$I$8))</f>
-        <v>346.5</v>
+        <v>303.75</v>
       </c>
     </row>
   </sheetData>
@@ -18367,6 +18367,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AG3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AH2:AW2"/>
     <mergeCell ref="AH3:AO3"/>
@@ -18375,14 +18383,6 @@
     <mergeCell ref="AX2:BM2"/>
     <mergeCell ref="AX3:BE3"/>
     <mergeCell ref="BF3:BM3"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19024,294 +19024,294 @@
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="60">
-        <v>5</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="60">
-        <v>5</v>
-      </c>
-      <c r="S3" s="61"/>
-      <c r="T3" s="61"/>
-      <c r="U3" s="61"/>
-      <c r="V3" s="61"/>
-      <c r="W3" s="61"/>
-      <c r="X3" s="61"/>
-      <c r="Y3" s="61"/>
-      <c r="Z3" s="61"/>
-      <c r="AA3" s="61"/>
-      <c r="AB3" s="61"/>
-      <c r="AC3" s="61"/>
-      <c r="AD3" s="61"/>
-      <c r="AE3" s="61"/>
-      <c r="AF3" s="61"/>
-      <c r="AG3" s="62"/>
-      <c r="AH3" s="60">
-        <v>5</v>
-      </c>
-      <c r="AI3" s="61"/>
-      <c r="AJ3" s="61"/>
-      <c r="AK3" s="61"/>
-      <c r="AL3" s="61"/>
-      <c r="AM3" s="61"/>
-      <c r="AN3" s="61"/>
-      <c r="AO3" s="61"/>
-      <c r="AP3" s="61"/>
-      <c r="AQ3" s="61"/>
-      <c r="AR3" s="61"/>
-      <c r="AS3" s="61"/>
-      <c r="AT3" s="61"/>
-      <c r="AU3" s="61"/>
-      <c r="AV3" s="61"/>
-      <c r="AW3" s="62"/>
-      <c r="AX3" s="60">
-        <v>5</v>
-      </c>
-      <c r="AY3" s="61"/>
-      <c r="AZ3" s="61"/>
-      <c r="BA3" s="61"/>
-      <c r="BB3" s="61"/>
-      <c r="BC3" s="61"/>
-      <c r="BD3" s="61"/>
-      <c r="BE3" s="61"/>
-      <c r="BF3" s="61"/>
-      <c r="BG3" s="61"/>
-      <c r="BH3" s="61"/>
-      <c r="BI3" s="61"/>
-      <c r="BJ3" s="61"/>
-      <c r="BK3" s="61"/>
-      <c r="BL3" s="61"/>
-      <c r="BM3" s="62"/>
-      <c r="BN3" s="60">
+      <c r="B3" s="63">
+        <v>5</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="63">
+        <v>5</v>
+      </c>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64"/>
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="65"/>
+      <c r="AH3" s="63">
+        <v>5</v>
+      </c>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64"/>
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64"/>
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64"/>
+      <c r="AV3" s="64"/>
+      <c r="AW3" s="65"/>
+      <c r="AX3" s="63">
+        <v>5</v>
+      </c>
+      <c r="AY3" s="64"/>
+      <c r="AZ3" s="64"/>
+      <c r="BA3" s="64"/>
+      <c r="BB3" s="64"/>
+      <c r="BC3" s="64"/>
+      <c r="BD3" s="64"/>
+      <c r="BE3" s="64"/>
+      <c r="BF3" s="64"/>
+      <c r="BG3" s="64"/>
+      <c r="BH3" s="64"/>
+      <c r="BI3" s="64"/>
+      <c r="BJ3" s="64"/>
+      <c r="BK3" s="64"/>
+      <c r="BL3" s="64"/>
+      <c r="BM3" s="65"/>
+      <c r="BN3" s="63">
         <v>9</v>
       </c>
-      <c r="BO3" s="61"/>
-      <c r="BP3" s="61"/>
-      <c r="BQ3" s="61"/>
-      <c r="BR3" s="61"/>
-      <c r="BS3" s="61"/>
-      <c r="BT3" s="61"/>
-      <c r="BU3" s="61"/>
-      <c r="BV3" s="61"/>
-      <c r="BW3" s="61"/>
-      <c r="BX3" s="61"/>
-      <c r="BY3" s="61"/>
-      <c r="BZ3" s="61"/>
-      <c r="CA3" s="61"/>
-      <c r="CB3" s="61"/>
-      <c r="CC3" s="62"/>
-      <c r="CD3" s="60">
+      <c r="BO3" s="64"/>
+      <c r="BP3" s="64"/>
+      <c r="BQ3" s="64"/>
+      <c r="BR3" s="64"/>
+      <c r="BS3" s="64"/>
+      <c r="BT3" s="64"/>
+      <c r="BU3" s="64"/>
+      <c r="BV3" s="64"/>
+      <c r="BW3" s="64"/>
+      <c r="BX3" s="64"/>
+      <c r="BY3" s="64"/>
+      <c r="BZ3" s="64"/>
+      <c r="CA3" s="64"/>
+      <c r="CB3" s="64"/>
+      <c r="CC3" s="65"/>
+      <c r="CD3" s="63">
         <v>9</v>
       </c>
-      <c r="CE3" s="61"/>
-      <c r="CF3" s="61"/>
-      <c r="CG3" s="61"/>
-      <c r="CH3" s="61"/>
-      <c r="CI3" s="61"/>
-      <c r="CJ3" s="61"/>
-      <c r="CK3" s="61"/>
-      <c r="CL3" s="61"/>
-      <c r="CM3" s="61"/>
-      <c r="CN3" s="61"/>
-      <c r="CO3" s="61"/>
-      <c r="CP3" s="61"/>
-      <c r="CQ3" s="61"/>
-      <c r="CR3" s="61"/>
-      <c r="CS3" s="62"/>
-      <c r="CT3" s="60">
+      <c r="CE3" s="64"/>
+      <c r="CF3" s="64"/>
+      <c r="CG3" s="64"/>
+      <c r="CH3" s="64"/>
+      <c r="CI3" s="64"/>
+      <c r="CJ3" s="64"/>
+      <c r="CK3" s="64"/>
+      <c r="CL3" s="64"/>
+      <c r="CM3" s="64"/>
+      <c r="CN3" s="64"/>
+      <c r="CO3" s="64"/>
+      <c r="CP3" s="64"/>
+      <c r="CQ3" s="64"/>
+      <c r="CR3" s="64"/>
+      <c r="CS3" s="65"/>
+      <c r="CT3" s="63">
         <v>9</v>
       </c>
-      <c r="CU3" s="61"/>
-      <c r="CV3" s="61"/>
-      <c r="CW3" s="61"/>
-      <c r="CX3" s="61"/>
-      <c r="CY3" s="61"/>
-      <c r="CZ3" s="61"/>
-      <c r="DA3" s="61"/>
-      <c r="DB3" s="61"/>
-      <c r="DC3" s="61"/>
-      <c r="DD3" s="61"/>
-      <c r="DE3" s="61"/>
-      <c r="DF3" s="61"/>
-      <c r="DG3" s="61"/>
-      <c r="DH3" s="61"/>
-      <c r="DI3" s="62"/>
-      <c r="DJ3" s="60">
+      <c r="CU3" s="64"/>
+      <c r="CV3" s="64"/>
+      <c r="CW3" s="64"/>
+      <c r="CX3" s="64"/>
+      <c r="CY3" s="64"/>
+      <c r="CZ3" s="64"/>
+      <c r="DA3" s="64"/>
+      <c r="DB3" s="64"/>
+      <c r="DC3" s="64"/>
+      <c r="DD3" s="64"/>
+      <c r="DE3" s="64"/>
+      <c r="DF3" s="64"/>
+      <c r="DG3" s="64"/>
+      <c r="DH3" s="64"/>
+      <c r="DI3" s="65"/>
+      <c r="DJ3" s="63">
         <v>9</v>
       </c>
-      <c r="DK3" s="61"/>
-      <c r="DL3" s="61"/>
-      <c r="DM3" s="61"/>
-      <c r="DN3" s="61"/>
-      <c r="DO3" s="61"/>
-      <c r="DP3" s="61"/>
-      <c r="DQ3" s="61"/>
-      <c r="DR3" s="61"/>
-      <c r="DS3" s="61"/>
-      <c r="DT3" s="61"/>
-      <c r="DU3" s="61"/>
-      <c r="DV3" s="61"/>
-      <c r="DW3" s="61"/>
-      <c r="DX3" s="61"/>
-      <c r="DY3" s="62"/>
-      <c r="DZ3" s="63">
+      <c r="DK3" s="64"/>
+      <c r="DL3" s="64"/>
+      <c r="DM3" s="64"/>
+      <c r="DN3" s="64"/>
+      <c r="DO3" s="64"/>
+      <c r="DP3" s="64"/>
+      <c r="DQ3" s="64"/>
+      <c r="DR3" s="64"/>
+      <c r="DS3" s="64"/>
+      <c r="DT3" s="64"/>
+      <c r="DU3" s="64"/>
+      <c r="DV3" s="64"/>
+      <c r="DW3" s="64"/>
+      <c r="DX3" s="64"/>
+      <c r="DY3" s="65"/>
+      <c r="DZ3" s="66">
         <v>13</v>
       </c>
-      <c r="EA3" s="64"/>
-      <c r="EB3" s="64"/>
-      <c r="EC3" s="64"/>
-      <c r="ED3" s="64"/>
-      <c r="EE3" s="64"/>
-      <c r="EF3" s="64"/>
-      <c r="EG3" s="64"/>
-      <c r="EH3" s="64"/>
-      <c r="EI3" s="64"/>
-      <c r="EJ3" s="64"/>
-      <c r="EK3" s="64"/>
-      <c r="EL3" s="64"/>
-      <c r="EM3" s="64"/>
-      <c r="EN3" s="64"/>
-      <c r="EO3" s="65"/>
-      <c r="EP3" s="66">
+      <c r="EA3" s="61"/>
+      <c r="EB3" s="61"/>
+      <c r="EC3" s="61"/>
+      <c r="ED3" s="61"/>
+      <c r="EE3" s="61"/>
+      <c r="EF3" s="61"/>
+      <c r="EG3" s="61"/>
+      <c r="EH3" s="61"/>
+      <c r="EI3" s="61"/>
+      <c r="EJ3" s="61"/>
+      <c r="EK3" s="61"/>
+      <c r="EL3" s="61"/>
+      <c r="EM3" s="61"/>
+      <c r="EN3" s="61"/>
+      <c r="EO3" s="62"/>
+      <c r="EP3" s="60">
         <v>13</v>
       </c>
-      <c r="EQ3" s="64"/>
-      <c r="ER3" s="64"/>
-      <c r="ES3" s="64"/>
-      <c r="ET3" s="64"/>
-      <c r="EU3" s="64"/>
-      <c r="EV3" s="64"/>
-      <c r="EW3" s="64"/>
-      <c r="EX3" s="64"/>
-      <c r="EY3" s="64"/>
-      <c r="EZ3" s="64"/>
-      <c r="FA3" s="64"/>
-      <c r="FB3" s="64"/>
-      <c r="FC3" s="64"/>
-      <c r="FD3" s="64"/>
-      <c r="FE3" s="65"/>
-      <c r="FF3" s="66">
+      <c r="EQ3" s="61"/>
+      <c r="ER3" s="61"/>
+      <c r="ES3" s="61"/>
+      <c r="ET3" s="61"/>
+      <c r="EU3" s="61"/>
+      <c r="EV3" s="61"/>
+      <c r="EW3" s="61"/>
+      <c r="EX3" s="61"/>
+      <c r="EY3" s="61"/>
+      <c r="EZ3" s="61"/>
+      <c r="FA3" s="61"/>
+      <c r="FB3" s="61"/>
+      <c r="FC3" s="61"/>
+      <c r="FD3" s="61"/>
+      <c r="FE3" s="62"/>
+      <c r="FF3" s="60">
         <v>13</v>
       </c>
-      <c r="FG3" s="64"/>
-      <c r="FH3" s="64"/>
-      <c r="FI3" s="64"/>
-      <c r="FJ3" s="64"/>
-      <c r="FK3" s="64"/>
-      <c r="FL3" s="64"/>
-      <c r="FM3" s="64"/>
-      <c r="FN3" s="64"/>
-      <c r="FO3" s="64"/>
-      <c r="FP3" s="64"/>
-      <c r="FQ3" s="64"/>
-      <c r="FR3" s="64"/>
-      <c r="FS3" s="64"/>
-      <c r="FT3" s="64"/>
-      <c r="FU3" s="65"/>
-      <c r="FV3" s="66">
+      <c r="FG3" s="61"/>
+      <c r="FH3" s="61"/>
+      <c r="FI3" s="61"/>
+      <c r="FJ3" s="61"/>
+      <c r="FK3" s="61"/>
+      <c r="FL3" s="61"/>
+      <c r="FM3" s="61"/>
+      <c r="FN3" s="61"/>
+      <c r="FO3" s="61"/>
+      <c r="FP3" s="61"/>
+      <c r="FQ3" s="61"/>
+      <c r="FR3" s="61"/>
+      <c r="FS3" s="61"/>
+      <c r="FT3" s="61"/>
+      <c r="FU3" s="62"/>
+      <c r="FV3" s="60">
         <v>13</v>
       </c>
-      <c r="FW3" s="64"/>
-      <c r="FX3" s="64"/>
-      <c r="FY3" s="64"/>
-      <c r="FZ3" s="64"/>
-      <c r="GA3" s="64"/>
-      <c r="GB3" s="64"/>
-      <c r="GC3" s="64"/>
-      <c r="GD3" s="64"/>
-      <c r="GE3" s="64"/>
-      <c r="GF3" s="64"/>
-      <c r="GG3" s="64"/>
-      <c r="GH3" s="64"/>
-      <c r="GI3" s="64"/>
-      <c r="GJ3" s="64"/>
-      <c r="GK3" s="65"/>
-      <c r="GL3" s="66">
+      <c r="FW3" s="61"/>
+      <c r="FX3" s="61"/>
+      <c r="FY3" s="61"/>
+      <c r="FZ3" s="61"/>
+      <c r="GA3" s="61"/>
+      <c r="GB3" s="61"/>
+      <c r="GC3" s="61"/>
+      <c r="GD3" s="61"/>
+      <c r="GE3" s="61"/>
+      <c r="GF3" s="61"/>
+      <c r="GG3" s="61"/>
+      <c r="GH3" s="61"/>
+      <c r="GI3" s="61"/>
+      <c r="GJ3" s="61"/>
+      <c r="GK3" s="62"/>
+      <c r="GL3" s="60">
         <v>17</v>
       </c>
-      <c r="GM3" s="64"/>
-      <c r="GN3" s="64"/>
-      <c r="GO3" s="64"/>
-      <c r="GP3" s="64"/>
-      <c r="GQ3" s="64"/>
-      <c r="GR3" s="64"/>
-      <c r="GS3" s="64"/>
-      <c r="GT3" s="64"/>
-      <c r="GU3" s="64"/>
-      <c r="GV3" s="64"/>
-      <c r="GW3" s="64"/>
-      <c r="GX3" s="64"/>
-      <c r="GY3" s="64"/>
-      <c r="GZ3" s="64"/>
-      <c r="HA3" s="65"/>
-      <c r="HB3" s="66">
+      <c r="GM3" s="61"/>
+      <c r="GN3" s="61"/>
+      <c r="GO3" s="61"/>
+      <c r="GP3" s="61"/>
+      <c r="GQ3" s="61"/>
+      <c r="GR3" s="61"/>
+      <c r="GS3" s="61"/>
+      <c r="GT3" s="61"/>
+      <c r="GU3" s="61"/>
+      <c r="GV3" s="61"/>
+      <c r="GW3" s="61"/>
+      <c r="GX3" s="61"/>
+      <c r="GY3" s="61"/>
+      <c r="GZ3" s="61"/>
+      <c r="HA3" s="62"/>
+      <c r="HB3" s="60">
         <v>17</v>
       </c>
-      <c r="HC3" s="64"/>
-      <c r="HD3" s="64"/>
-      <c r="HE3" s="64"/>
-      <c r="HF3" s="64"/>
-      <c r="HG3" s="64"/>
-      <c r="HH3" s="64"/>
-      <c r="HI3" s="64"/>
-      <c r="HJ3" s="64"/>
-      <c r="HK3" s="64"/>
-      <c r="HL3" s="64"/>
-      <c r="HM3" s="64"/>
-      <c r="HN3" s="64"/>
-      <c r="HO3" s="64"/>
-      <c r="HP3" s="64"/>
-      <c r="HQ3" s="65"/>
-      <c r="HR3" s="66">
+      <c r="HC3" s="61"/>
+      <c r="HD3" s="61"/>
+      <c r="HE3" s="61"/>
+      <c r="HF3" s="61"/>
+      <c r="HG3" s="61"/>
+      <c r="HH3" s="61"/>
+      <c r="HI3" s="61"/>
+      <c r="HJ3" s="61"/>
+      <c r="HK3" s="61"/>
+      <c r="HL3" s="61"/>
+      <c r="HM3" s="61"/>
+      <c r="HN3" s="61"/>
+      <c r="HO3" s="61"/>
+      <c r="HP3" s="61"/>
+      <c r="HQ3" s="62"/>
+      <c r="HR3" s="60">
         <v>17</v>
       </c>
-      <c r="HS3" s="64"/>
-      <c r="HT3" s="64"/>
-      <c r="HU3" s="64"/>
-      <c r="HV3" s="64"/>
-      <c r="HW3" s="64"/>
-      <c r="HX3" s="64"/>
-      <c r="HY3" s="64"/>
-      <c r="HZ3" s="64"/>
-      <c r="IA3" s="64"/>
-      <c r="IB3" s="64"/>
-      <c r="IC3" s="64"/>
-      <c r="ID3" s="64"/>
-      <c r="IE3" s="64"/>
-      <c r="IF3" s="64"/>
-      <c r="IG3" s="65"/>
-      <c r="IH3" s="66">
+      <c r="HS3" s="61"/>
+      <c r="HT3" s="61"/>
+      <c r="HU3" s="61"/>
+      <c r="HV3" s="61"/>
+      <c r="HW3" s="61"/>
+      <c r="HX3" s="61"/>
+      <c r="HY3" s="61"/>
+      <c r="HZ3" s="61"/>
+      <c r="IA3" s="61"/>
+      <c r="IB3" s="61"/>
+      <c r="IC3" s="61"/>
+      <c r="ID3" s="61"/>
+      <c r="IE3" s="61"/>
+      <c r="IF3" s="61"/>
+      <c r="IG3" s="62"/>
+      <c r="IH3" s="60">
         <v>17</v>
       </c>
-      <c r="II3" s="64"/>
-      <c r="IJ3" s="64"/>
-      <c r="IK3" s="64"/>
-      <c r="IL3" s="64"/>
-      <c r="IM3" s="64"/>
-      <c r="IN3" s="64"/>
-      <c r="IO3" s="64"/>
-      <c r="IP3" s="64"/>
-      <c r="IQ3" s="64"/>
-      <c r="IR3" s="64"/>
-      <c r="IS3" s="64"/>
-      <c r="IT3" s="64"/>
-      <c r="IU3" s="64"/>
-      <c r="IV3" s="64"/>
-      <c r="IW3" s="65"/>
+      <c r="II3" s="61"/>
+      <c r="IJ3" s="61"/>
+      <c r="IK3" s="61"/>
+      <c r="IL3" s="61"/>
+      <c r="IM3" s="61"/>
+      <c r="IN3" s="61"/>
+      <c r="IO3" s="61"/>
+      <c r="IP3" s="61"/>
+      <c r="IQ3" s="61"/>
+      <c r="IR3" s="61"/>
+      <c r="IS3" s="61"/>
+      <c r="IT3" s="61"/>
+      <c r="IU3" s="61"/>
+      <c r="IV3" s="61"/>
+      <c r="IW3" s="62"/>
     </row>
     <row r="4" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -30012,19 +30012,57 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="HB2:HQ2"/>
-    <mergeCell ref="HR2:IG2"/>
-    <mergeCell ref="IH2:IW2"/>
-    <mergeCell ref="DZ2:EO2"/>
-    <mergeCell ref="EP2:FE2"/>
-    <mergeCell ref="FF2:FU2"/>
-    <mergeCell ref="FV2:GK2"/>
-    <mergeCell ref="GL2:HA2"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="BN2:CC2"/>
-    <mergeCell ref="CD2:CS2"/>
-    <mergeCell ref="CT2:DI2"/>
-    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AH4:AO4"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="BN4:BU4"/>
+    <mergeCell ref="BV4:CC4"/>
+    <mergeCell ref="CD4:CK4"/>
+    <mergeCell ref="CL4:CS4"/>
+    <mergeCell ref="CT4:DA4"/>
+    <mergeCell ref="DB4:DI4"/>
+    <mergeCell ref="DJ4:DQ4"/>
+    <mergeCell ref="DR4:DY4"/>
+    <mergeCell ref="DZ4:EG4"/>
+    <mergeCell ref="EH4:EO4"/>
+    <mergeCell ref="EP4:EW4"/>
+    <mergeCell ref="EX4:FE4"/>
+    <mergeCell ref="FF4:FM4"/>
+    <mergeCell ref="FN4:FU4"/>
+    <mergeCell ref="FV4:GC4"/>
+    <mergeCell ref="GD4:GK4"/>
+    <mergeCell ref="GL4:GS4"/>
+    <mergeCell ref="GT4:HA4"/>
+    <mergeCell ref="HB4:HI4"/>
+    <mergeCell ref="HJ4:HQ4"/>
+    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="HZ4:IG4"/>
+    <mergeCell ref="IH4:IO4"/>
+    <mergeCell ref="IP4:IW4"/>
+    <mergeCell ref="AH3:AW3"/>
+    <mergeCell ref="AX3:BM3"/>
+    <mergeCell ref="BN3:CC3"/>
+    <mergeCell ref="CD3:CS3"/>
+    <mergeCell ref="CT3:DI3"/>
+    <mergeCell ref="DJ3:DY3"/>
+    <mergeCell ref="DZ3:EO3"/>
+    <mergeCell ref="EP3:FE3"/>
+    <mergeCell ref="FF3:FU3"/>
+    <mergeCell ref="FV3:GK3"/>
+    <mergeCell ref="GL3:HA3"/>
+    <mergeCell ref="HB3:HQ3"/>
+    <mergeCell ref="HR3:IG3"/>
     <mergeCell ref="IH3:IW3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AX1:BM1"/>
@@ -30041,57 +30079,19 @@
     <mergeCell ref="HR1:IG1"/>
     <mergeCell ref="IH1:IW1"/>
     <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="HZ4:IG4"/>
-    <mergeCell ref="IH4:IO4"/>
-    <mergeCell ref="IP4:IW4"/>
-    <mergeCell ref="AH3:AW3"/>
-    <mergeCell ref="AX3:BM3"/>
-    <mergeCell ref="BN3:CC3"/>
-    <mergeCell ref="CD3:CS3"/>
-    <mergeCell ref="CT3:DI3"/>
-    <mergeCell ref="DJ3:DY3"/>
-    <mergeCell ref="DZ3:EO3"/>
-    <mergeCell ref="EP3:FE3"/>
-    <mergeCell ref="FF3:FU3"/>
-    <mergeCell ref="FV3:GK3"/>
-    <mergeCell ref="GL3:HA3"/>
-    <mergeCell ref="HB3:HQ3"/>
-    <mergeCell ref="HR3:IG3"/>
-    <mergeCell ref="GL4:GS4"/>
-    <mergeCell ref="GT4:HA4"/>
-    <mergeCell ref="HB4:HI4"/>
-    <mergeCell ref="HJ4:HQ4"/>
-    <mergeCell ref="HR4:HY4"/>
-    <mergeCell ref="EX4:FE4"/>
-    <mergeCell ref="FF4:FM4"/>
-    <mergeCell ref="FN4:FU4"/>
-    <mergeCell ref="FV4:GC4"/>
-    <mergeCell ref="GD4:GK4"/>
-    <mergeCell ref="DJ4:DQ4"/>
-    <mergeCell ref="DR4:DY4"/>
-    <mergeCell ref="DZ4:EG4"/>
-    <mergeCell ref="EH4:EO4"/>
-    <mergeCell ref="EP4:EW4"/>
-    <mergeCell ref="BV4:CC4"/>
-    <mergeCell ref="CD4:CK4"/>
-    <mergeCell ref="CL4:CS4"/>
-    <mergeCell ref="CT4:DA4"/>
-    <mergeCell ref="DB4:DI4"/>
-    <mergeCell ref="AH4:AO4"/>
-    <mergeCell ref="AP4:AW4"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="BF4:BM4"/>
-    <mergeCell ref="BN4:BU4"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="BN2:CC2"/>
+    <mergeCell ref="CD2:CS2"/>
+    <mergeCell ref="CT2:DI2"/>
+    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="HB2:HQ2"/>
+    <mergeCell ref="HR2:IG2"/>
+    <mergeCell ref="IH2:IW2"/>
+    <mergeCell ref="DZ2:EO2"/>
+    <mergeCell ref="EP2:FE2"/>
+    <mergeCell ref="FF2:FU2"/>
+    <mergeCell ref="FV2:GK2"/>
+    <mergeCell ref="GL2:HA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>